<commit_message>
update 25 March numbers
</commit_message>
<xml_diff>
--- a/COVID19 calculos.xlsx
+++ b/COVID19 calculos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rramirez/projects/git-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E25EE6E-CD10-0948-9DE1-249BB1CB6FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86934029-5E76-6042-B108-BB6F00E29D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
+    <workbookView xWindow="360" yWindow="600" windowWidth="28800" windowHeight="16540" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculos COVID19" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>China</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>23 March</t>
+  </si>
+  <si>
+    <t>24 March</t>
   </si>
 </sst>
 </file>
@@ -318,10 +321,10 @@
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Spain</c:v>
@@ -342,10 +345,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Sweden</c:v>
@@ -360,10 +363,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Canada</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Colombia</c:v>
@@ -378,10 +381,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>800.81680280046669</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>885.87962962962968</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>800.81680280046669</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>546.42091727389629</c:v>
@@ -402,10 +405,10 @@
                   <c:v>215.83818480370206</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>211.35040745052387</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>253.94282897979301</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>211.35040745052387</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>174.901185770751</c:v>
@@ -420,10 +423,10 @@
                   <c:v>75.526791089705</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>35.328544825751528</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>58.447330447330444</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>35.328544825751528</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>3.9942938659058487</c:v>
@@ -467,10 +470,10 @@
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Spain</c:v>
@@ -491,10 +494,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Sweden</c:v>
@@ -509,10 +512,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Canada</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Colombia</c:v>
@@ -527,10 +530,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>872.11201866977831</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>977.81084656084658</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>872.11201866977831</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>613.00900128589808</c:v>
@@ -551,10 +554,10 @@
                   <c:v>239</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>267</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>191</c:v>
@@ -569,10 +572,10 @@
                   <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>5</c:v>
@@ -616,10 +619,10 @@
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Spain</c:v>
@@ -640,10 +643,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Sweden</c:v>
@@ -658,10 +661,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Canada</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>Colombia</c:v>
@@ -676,10 +679,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>997</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1057</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>997</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>709</c:v>
@@ -700,10 +703,10 @@
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>202</c:v>
@@ -717,11 +720,11 @@
                 <c:pt idx="13">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0">
+                <c:pt idx="14">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0">
                   <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>6</c:v>
@@ -732,6 +735,155 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-30B0-1341-8564-275AF7CEB475}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$E$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>24 March</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$22:$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$E$22:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1144</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>518</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E4A6-FA42-ADDC-2F07F0000D6D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1086,13 +1238,13 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Switzerland</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Belgium</c:v>
@@ -1101,16 +1253,16 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sweden</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Austria</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Norway</c:v>
@@ -1146,13 +1298,13 @@
                   <c:v>19.172005914243471</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>8.3893118375876998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9161816065192081</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>9.3348891481913654</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.3893118375876998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.9161816065192081</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5.8771929824561404</c:v>
@@ -1161,16 +1313,16 @@
                   <c:v>3.5069235400361229</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>1.9762845849802373</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90702947845804982</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2.3484848484848486</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>1.9817369341363902</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.9762845849802373</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.90702947845804982</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1.3040238450074515</c:v>
@@ -1235,13 +1387,13 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Switzerland</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Belgium</c:v>
@@ -1250,16 +1402,16 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sweden</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Austria</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Norway</c:v>
@@ -1295,13 +1447,13 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>7</c:v>
@@ -1384,13 +1536,13 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Switzerland</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Belgium</c:v>
@@ -1399,16 +1551,16 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Sweden</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Austria</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Norway</c:v>
@@ -1444,13 +1596,13 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>8</c:v>
@@ -1491,6 +1643,155 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7493-3441-8635-D8D4141158B0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$E$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>24 March</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$57:$A$73</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$E$57:$E$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F899-1742-8A20-7614E15055DB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3159,8 +3460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3BD7B-3B40-A94B-99F4-AAD0A2BEB996}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3199,24 +3500,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>81093</v>
+        <v>81171</v>
       </c>
       <c r="C2" s="2">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2">
-        <v>3270</v>
+        <v>3277</v>
       </c>
       <c r="E2" s="3">
         <v>1386</v>
       </c>
       <c r="F2" s="5">
         <f>B2/E2</f>
-        <v>58.50865800865801</v>
+        <v>58.564935064935064</v>
       </c>
       <c r="G2" s="5">
         <f>D2/E2</f>
-        <v>2.3593073593073592</v>
+        <v>2.3643578643578644</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -3226,24 +3527,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>63927</v>
+        <v>69176</v>
       </c>
       <c r="C3" s="2">
-        <v>4789</v>
+        <v>5249</v>
       </c>
       <c r="D3" s="2">
-        <v>6077</v>
+        <v>6820</v>
       </c>
       <c r="E3" s="4">
         <v>60.48</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F18" si="0">B3/E3</f>
-        <v>1056.9940476190477</v>
+        <v>1143.7830687830688</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G18" si="1">D3/E3</f>
-        <v>100.47949735449735</v>
+        <v>112.76455026455027</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -3253,24 +3554,24 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>33089</v>
+        <v>39885</v>
       </c>
       <c r="C4" s="2">
-        <v>4321</v>
+        <v>4749</v>
       </c>
       <c r="D4" s="2">
-        <v>2207</v>
+        <v>2808</v>
       </c>
       <c r="E4" s="4">
         <v>46.66</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="0"/>
-        <v>709.15130732961859</v>
+        <v>854.80068581225896</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="1"/>
-        <v>47.299614230604377</v>
+        <v>60.180025717959715</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -3280,24 +3581,24 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>42163</v>
+        <v>52983</v>
       </c>
       <c r="C5" s="2">
-        <v>8617</v>
+        <v>9249</v>
       </c>
       <c r="D5" s="2">
-        <v>512</v>
+        <v>685</v>
       </c>
       <c r="E5" s="4">
         <v>327.2</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>128.86002444987776</v>
+        <v>161.92848410757946</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" si="1"/>
-        <v>1.5647921760391199</v>
+        <f>D5/E5</f>
+        <v>2.0935207823960882</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -3307,24 +3608,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>29056</v>
+        <v>32986</v>
       </c>
       <c r="C6" s="2">
-        <v>4183</v>
+        <v>3903</v>
       </c>
       <c r="D6" s="2">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="E6" s="4">
         <v>82.79</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>350.960260901075</v>
+        <v>398.42976204855654</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>1.4252929097717115</v>
+        <v>1.8963642952047348</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -3334,24 +3635,24 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>23049</v>
+        <v>24811</v>
       </c>
       <c r="C7" s="2">
-        <v>1411</v>
+        <v>1762</v>
       </c>
       <c r="D7" s="2">
-        <v>1812</v>
+        <v>1934</v>
       </c>
       <c r="E7" s="4">
         <v>81.16</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>283.99457861015281</v>
+        <v>305.70478068013801</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="1"/>
-        <v>22.326269098077873</v>
+        <v>23.829472646623955</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -3361,24 +3662,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>19856</v>
+        <v>22304</v>
       </c>
       <c r="C8" s="2">
-        <v>3838</v>
+        <v>2448</v>
       </c>
       <c r="D8" s="2">
-        <v>860</v>
+        <v>1100</v>
       </c>
       <c r="E8" s="4">
         <v>66.989999999999995</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>296.40244812658608</v>
+        <v>332.94521570383642</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="1"/>
-        <v>12.837736975668012</v>
+        <v>16.420361247947454</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3388,24 +3689,24 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>8961</v>
+        <v>9037</v>
       </c>
       <c r="C9" s="2">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D9" s="2">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E9" s="4">
         <v>51.47</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>174.10141830192345</v>
+        <v>175.5780066057898</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>2.1565960753837188</v>
+        <v>2.3314552166310474</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -3415,24 +3716,24 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>8547</v>
+        <v>9877</v>
       </c>
       <c r="C10" s="2">
-        <v>1073</v>
+        <v>1082</v>
       </c>
       <c r="D10" s="2">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E10" s="4">
         <v>8.57</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>997.31621936989495</v>
+        <v>1152.5087514585764</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>13.768961493582264</v>
+        <v>14.235705950991832</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3442,24 +3743,24 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>6650</v>
+        <v>8077</v>
       </c>
       <c r="C11" s="2">
-        <v>967</v>
+        <v>1427</v>
       </c>
       <c r="D11" s="2">
-        <v>335</v>
+        <v>422</v>
       </c>
       <c r="E11" s="4">
         <v>66.44</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>100.09030704394944</v>
+        <v>121.56833232992174</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="1"/>
-        <v>5.0421432871764003</v>
+        <v>6.351595424443107</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3469,24 +3770,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>4749</v>
+        <v>5560</v>
       </c>
       <c r="C12" s="2">
-        <v>545</v>
+        <v>811</v>
       </c>
       <c r="D12" s="2">
-        <v>213</v>
+        <v>276</v>
       </c>
       <c r="E12" s="4">
         <v>17.18</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>276.42607683352736</v>
+        <v>323.63213038416762</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="1"/>
-        <v>12.39813736903376</v>
+        <v>16.065192083818395</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -3496,24 +3797,24 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>4468</v>
+        <v>5283</v>
       </c>
       <c r="C13" s="2">
-        <v>886</v>
+        <v>809</v>
       </c>
       <c r="D13" s="2">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E13" s="4">
         <v>8.82</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>506.57596371882084</v>
+        <v>598.9795918367347</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="1"/>
-        <v>2.3809523809523809</v>
+        <v>3.1746031746031744</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3523,24 +3824,24 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>3743</v>
+        <v>4269</v>
       </c>
       <c r="C14" s="2">
-        <v>342</v>
+        <v>526</v>
       </c>
       <c r="D14" s="2">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="E14" s="4">
         <v>11.4</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>328.33333333333331</v>
+        <v>374.4736842105263</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="1"/>
-        <v>7.7192982456140351</v>
+        <v>10.701754385964913</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -3550,24 +3851,24 @@
         <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>2547</v>
+        <v>2779</v>
       </c>
       <c r="C15" s="2">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D15" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4">
         <v>5.3680000000000003</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="0"/>
-        <v>474.47839046199698</v>
+        <v>517.69746646795829</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="1"/>
-        <v>1.8628912071535022</v>
+        <v>2.2354694485842024</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3575,24 +3876,24 @@
         <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>2046</v>
+        <v>2286</v>
       </c>
       <c r="C16" s="2">
-        <v>112</v>
+        <v>240</v>
       </c>
       <c r="D16" s="2">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4">
         <v>10.119999999999999</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>202.17391304347828</v>
+        <v>225.88932806324112</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="1"/>
-        <v>2.4703557312252968</v>
+        <v>3.5573122529644272</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3602,24 +3903,24 @@
         <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>2035</v>
+        <v>2590</v>
       </c>
       <c r="C17" s="2">
-        <v>565</v>
+        <v>499</v>
       </c>
       <c r="D17" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E17" s="4">
         <v>37.590000000000003</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>54.136738494280387</v>
+        <v>68.901303538175043</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="1"/>
-        <v>0.6118648576749135</v>
+        <v>0.66507049747273206</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -3627,10 +3928,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>277</v>
+        <v>306</v>
       </c>
       <c r="C18" s="2">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -3640,7 +3941,7 @@
       </c>
       <c r="F18" s="5">
         <f t="shared" si="0"/>
-        <v>5.6449969431424494</v>
+        <v>6.235989402893825</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="1"/>
@@ -3648,9 +3949,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E19" s="4">
-        <v>10</v>
-      </c>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
@@ -3669,33 +3968,42 @@
       <c r="D21" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="E21" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B22" s="5">
-        <v>885.87962962962968</v>
+        <v>800.81680280046669</v>
       </c>
       <c r="C22" s="5">
-        <v>977.81084656084658</v>
+        <v>872.11201866977831</v>
       </c>
       <c r="D22">
-        <v>1057</v>
+        <v>997</v>
+      </c>
+      <c r="E22">
+        <v>1153</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B23" s="5">
-        <v>800.81680280046669</v>
+        <v>885.87962962962968</v>
       </c>
       <c r="C23" s="5">
-        <v>872.11201866977831</v>
+        <v>977.81084656084658</v>
       </c>
       <c r="D23">
-        <v>997</v>
+        <v>1057</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1144</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -3711,6 +4019,9 @@
       <c r="D24">
         <v>709</v>
       </c>
+      <c r="E24">
+        <v>855</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -3725,6 +4036,9 @@
       <c r="D25">
         <v>507</v>
       </c>
+      <c r="E25">
+        <v>599</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -3739,6 +4053,9 @@
       <c r="D26">
         <v>474</v>
       </c>
+      <c r="E26">
+        <v>518</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -3753,6 +4070,9 @@
       <c r="D27">
         <v>351</v>
       </c>
+      <c r="E27">
+        <v>398</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -3767,6 +4087,9 @@
       <c r="D28">
         <v>328</v>
       </c>
+      <c r="E28">
+        <v>374</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -3781,33 +4104,42 @@
       <c r="D29">
         <v>296</v>
       </c>
+      <c r="E29">
+        <v>333</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B30" s="5">
-        <v>253.94282897979301</v>
+        <v>211.35040745052387</v>
       </c>
       <c r="C30" s="5">
-        <v>267</v>
+        <v>245</v>
       </c>
       <c r="D30">
-        <v>284</v>
+        <v>276</v>
+      </c>
+      <c r="E30">
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B31" s="5">
-        <v>211.35040745052387</v>
+        <v>253.94282897979301</v>
       </c>
       <c r="C31" s="5">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D31">
-        <v>276</v>
+        <v>284</v>
+      </c>
+      <c r="E31">
+        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -3823,8 +4155,11 @@
       <c r="D32">
         <v>202</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -3837,8 +4172,11 @@
       <c r="D33">
         <v>174</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -3851,8 +4189,11 @@
       <c r="D34">
         <v>129</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -3865,36 +4206,45 @@
       <c r="D35">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="5">
+        <v>35.328544825751528</v>
+      </c>
+      <c r="C36" s="5">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>54</v>
+      </c>
+      <c r="E36">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B37" s="5">
         <v>58.447330447330444</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>58</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D37" s="5">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="5">
-        <v>35.328544825751528</v>
-      </c>
-      <c r="C37" s="5">
-        <v>38</v>
-      </c>
-      <c r="D37">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -3907,8 +4257,11 @@
       <c r="D38">
         <v>6</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -3921,8 +4274,11 @@
       <c r="D56" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>1</v>
       </c>
@@ -3935,8 +4291,11 @@
       <c r="D57">
         <v>100</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>2</v>
       </c>
@@ -3949,8 +4308,11 @@
       <c r="D58">
         <v>47</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -3963,50 +4325,62 @@
       <c r="D59">
         <v>22</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B60" s="5">
-        <v>9.3348891481913654</v>
+        <v>8.3893118375876998</v>
       </c>
       <c r="C60">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="E60">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B61" s="5">
-        <v>8.3893118375876998</v>
+        <v>7.9161816065192081</v>
       </c>
       <c r="C61">
         <v>10</v>
       </c>
       <c r="D61">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E61">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B62" s="5">
-        <v>7.9161816065192081</v>
+        <v>9.3348891481913654</v>
       </c>
       <c r="C62">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D62">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="E62">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>12</v>
       </c>
@@ -4019,8 +4393,11 @@
       <c r="D63">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>9</v>
       </c>
@@ -4033,13 +4410,16 @@
       <c r="D64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B65" s="5">
-        <v>2.3484848484848486</v>
+        <v>1.9762845849802373</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -4047,13 +4427,16 @@
       <c r="D65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B66" s="5">
-        <v>1.9817369341363902</v>
+        <v>0.90702947845804982</v>
       </c>
       <c r="C66">
         <v>2</v>
@@ -4061,13 +4444,16 @@
       <c r="D66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B67" s="5">
-        <v>1.9762845849802373</v>
+        <v>2.3484848484848486</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -4075,13 +4461,16 @@
       <c r="D67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B68" s="5">
-        <v>0.90702947845804982</v>
+        <v>1.9817369341363902</v>
       </c>
       <c r="C68">
         <v>2</v>
@@ -4089,8 +4478,11 @@
       <c r="D68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>19</v>
       </c>
@@ -4103,8 +4495,11 @@
       <c r="D69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>3</v>
       </c>
@@ -4117,8 +4512,11 @@
       <c r="D70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -4131,8 +4529,11 @@
       <c r="D71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>21</v>
       </c>
@@ -4145,8 +4546,11 @@
       <c r="D72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>22</v>
       </c>
@@ -4159,10 +4563,13 @@
       <c r="D73">
         <v>0</v>
       </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A57:D73">
-    <sortCondition descending="1" ref="D57:D73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A57:E73">
+    <sortCondition descending="1" ref="E57:E73"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B20:C20"/>
@@ -4184,37 +4591,37 @@
     <hyperlink ref="A15" r:id="rId14" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{EFD81247-2449-C842-A355-C3CA98069F0C}"/>
     <hyperlink ref="A16" r:id="rId15" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{6A5FA689-4530-FC48-8476-8EB82E5F1FB4}"/>
     <hyperlink ref="A17" r:id="rId16" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{768069AF-3C8F-EA44-BDE0-CFAD42D2AE89}"/>
-    <hyperlink ref="A36" r:id="rId17" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{2749059A-A8E1-B840-90D7-560A71410172}"/>
-    <hyperlink ref="A22" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
+    <hyperlink ref="A37" r:id="rId17" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{2749059A-A8E1-B840-90D7-560A71410172}"/>
+    <hyperlink ref="A23" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
     <hyperlink ref="A24" r:id="rId19" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{57A3EA1C-224C-3F47-BBF4-F96842A83158}"/>
     <hyperlink ref="A34" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
     <hyperlink ref="A27" r:id="rId21" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{AB6442DB-502D-BF47-BD97-FD78208EA473}"/>
-    <hyperlink ref="A30" r:id="rId22" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{E8933148-C5A5-C049-998E-8A19BCC472EE}"/>
+    <hyperlink ref="A31" r:id="rId22" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{E8933148-C5A5-C049-998E-8A19BCC472EE}"/>
     <hyperlink ref="A29" r:id="rId23" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{148898F7-DFEC-AD49-AE18-589CAE84737B}"/>
     <hyperlink ref="A33" r:id="rId24" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{C028FE55-7852-3F41-9817-549C985F7260}"/>
-    <hyperlink ref="A23" r:id="rId25" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{B5BDCE1C-B9BF-5D4E-AF41-63D149E1115B}"/>
+    <hyperlink ref="A22" r:id="rId25" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{B5BDCE1C-B9BF-5D4E-AF41-63D149E1115B}"/>
     <hyperlink ref="A35" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
-    <hyperlink ref="A31" r:id="rId27" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{D6541E56-79D1-DD4C-89C0-B9FE943CF17D}"/>
+    <hyperlink ref="A30" r:id="rId27" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{D6541E56-79D1-DD4C-89C0-B9FE943CF17D}"/>
     <hyperlink ref="A25" r:id="rId28" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{DB82E052-EA56-4542-B5D9-CDCA3F75C63F}"/>
     <hyperlink ref="A28" r:id="rId29" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{B76E0484-5117-5040-B058-D17B21DC5420}"/>
     <hyperlink ref="A26" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
     <hyperlink ref="A32" r:id="rId31" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{219CBCE6-9D2C-5146-B0CA-29FE2A0FA513}"/>
-    <hyperlink ref="A37" r:id="rId32" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{A66187B1-4AD9-444B-BCFA-FF8464EDFF33}"/>
-    <hyperlink ref="A65" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
+    <hyperlink ref="A36" r:id="rId32" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{A66187B1-4AD9-444B-BCFA-FF8464EDFF33}"/>
+    <hyperlink ref="A67" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
     <hyperlink ref="A57" r:id="rId34" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{A20FB0CD-F9DA-914E-B2F5-F280E65964E3}"/>
     <hyperlink ref="A58" r:id="rId35" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{EE62FA68-128F-064D-A4F8-F9BE8B79FC59}"/>
     <hyperlink ref="A70" r:id="rId36" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{D2FB73FA-EC57-274E-BF29-C09B1AC3DDE2}"/>
     <hyperlink ref="A71" r:id="rId37" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{523B8969-55CC-FF4F-9FA9-106BC6D662B5}"/>
     <hyperlink ref="A59" r:id="rId38" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{517487C3-ADE3-274F-9F6E-78AC36F61827}"/>
-    <hyperlink ref="A61" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
-    <hyperlink ref="A66" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
-    <hyperlink ref="A60" r:id="rId41" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{92D1F4A4-B981-3C45-A55A-E63BE05C7D4F}"/>
+    <hyperlink ref="A60" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
+    <hyperlink ref="A68" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
+    <hyperlink ref="A62" r:id="rId41" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{92D1F4A4-B981-3C45-A55A-E63BE05C7D4F}"/>
     <hyperlink ref="A64" r:id="rId42" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{9E857743-3BA1-D547-A532-A53EF891F862}"/>
-    <hyperlink ref="A62" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
-    <hyperlink ref="A68" r:id="rId44" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{76C0B263-3E56-DD44-BF90-D7A725F4C11B}"/>
+    <hyperlink ref="A61" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
+    <hyperlink ref="A66" r:id="rId44" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{76C0B263-3E56-DD44-BF90-D7A725F4C11B}"/>
     <hyperlink ref="A63" r:id="rId45" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{F788A2F0-F76C-0A46-84F6-32311CDCE6EB}"/>
     <hyperlink ref="A69" r:id="rId46" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{1FA4FB2B-21FB-A240-B716-855DE4CC3FCA}"/>
-    <hyperlink ref="A67" r:id="rId47" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{52773F30-B0DE-FE41-B798-80BFDD6B52F9}"/>
+    <hyperlink ref="A65" r:id="rId47" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{52773F30-B0DE-FE41-B798-80BFDD6B52F9}"/>
     <hyperlink ref="A72" r:id="rId48" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{03FEC42E-DDC8-9B40-8CF7-F008D15BED91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Denmark added as country
</commit_message>
<xml_diff>
--- a/COVID19 calculos.xlsx
+++ b/COVID19 calculos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rramirez/projects/git-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86934029-5E76-6042-B108-BB6F00E29D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA75E01-B8B3-2F49-A035-D6062D7BFB62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="600" windowWidth="28800" windowHeight="16540" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
+    <workbookView xWindow="3520" yWindow="980" windowWidth="37020" windowHeight="17380" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculos COVID19" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t>China</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>24 March</t>
+  </si>
+  <si>
+    <t>Denmark</t>
   </si>
 </sst>
 </file>
@@ -296,7 +299,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$B$21</c:f>
+              <c:f>'Calculos COVID19'!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -317,9 +320,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$22:$A$38</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -351,24 +354,27 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>UK</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -376,10 +382,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$B$22:$B$38</c:f>
+              <c:f>'Calculos COVID19'!$B$27:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>800.81680280046669</c:v>
                 </c:pt>
@@ -411,24 +417,27 @@
                   <c:v>253.94282897979301</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>174.901185770751</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>170.95395375947155</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>73.67053789731051</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>75.526791089705</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>35.328544825751528</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>58.447330447330444</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>3.9942938659058487</c:v>
                 </c:pt>
               </c:numCache>
@@ -445,7 +454,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$C$21</c:f>
+              <c:f>'Calculos COVID19'!$C$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -466,9 +475,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$22:$A$38</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -500,24 +509,27 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>UK</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -525,10 +537,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$C$22:$C$38</c:f>
+              <c:f>'Calculos COVID19'!$C$27:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>872.11201866977831</c:v>
                 </c:pt>
@@ -560,24 +572,27 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>191</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>173</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>99</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -594,7 +609,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$D$21</c:f>
+              <c:f>'Calculos COVID19'!$D$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -615,9 +630,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$22:$A$38</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -649,24 +664,27 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>UK</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -674,10 +692,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$D$22:$D$38</c:f>
+              <c:f>'Calculos COVID19'!$D$27:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>997</c:v>
                 </c:pt>
@@ -709,24 +727,27 @@
                   <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>202</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>174</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>129</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="0">
+                <c:pt idx="16" formatCode="0">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -743,7 +764,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$E$21</c:f>
+              <c:f>'Calculos COVID19'!$E$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -764,9 +785,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$22:$A$38</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -798,24 +819,27 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>UK</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -823,10 +847,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$E$22:$E$38</c:f>
+              <c:f>'Calculos COVID19'!$E$27:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>1153</c:v>
                 </c:pt>
@@ -858,24 +882,27 @@
                   <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
                   <c:v>226</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="12" formatCode="General">
                   <c:v>176</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="13" formatCode="General">
                   <c:v>162</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="14" formatCode="General">
                   <c:v>122</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="15" formatCode="General">
                   <c:v>69</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="17" formatCode="General">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -1204,7 +1231,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$B$56</c:f>
+              <c:f>'Calculos COVID19'!$B$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1225,9 +1252,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$57:$A$73</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1253,30 +1280,33 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Austria</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Norway</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Germany</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -1284,10 +1314,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$B$57:$B$73</c:f>
+              <c:f>'Calculos COVID19'!$B$62:$B$79</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>79.778439153439152</c:v>
                 </c:pt>
@@ -1313,30 +1343,33 @@
                   <c:v>3.5069235400361229</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>1.9762845849802373</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.90702947845804982</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>2.3484848484848486</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>1.9817369341363902</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1.3040238450074515</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>0.91992665036674814</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1.0146152917018962</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>0.50545357807927638</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1353,7 +1386,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$C$56</c:f>
+              <c:f>'Calculos COVID19'!$C$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1374,9 +1407,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$57:$A$73</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1402,30 +1435,33 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Austria</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Norway</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Germany</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -1433,10 +1469,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$C$57:$C$73</c:f>
+              <c:f>'Calculos COVID19'!$C$62:$C$79</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>90.542328042328052</c:v>
                 </c:pt>
@@ -1462,7 +1498,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>2</c:v>
@@ -1474,7 +1510,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
                   <c:v>1</c:v>
@@ -1486,6 +1522,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1502,7 +1541,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$D$56</c:f>
+              <c:f>'Calculos COVID19'!$D$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1523,9 +1562,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$57:$A$73</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1551,30 +1590,33 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Austria</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Norway</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Germany</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -1582,10 +1624,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$D$57:$D$73</c:f>
+              <c:f>'Calculos COVID19'!$D$62:$D$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -1611,7 +1653,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2</c:v>
@@ -1629,12 +1671,15 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1651,7 +1696,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$E$56</c:f>
+              <c:f>'Calculos COVID19'!$E$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1672,9 +1717,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$57:$A$73</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1700,30 +1745,33 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Sweden</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Austria</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>S. Korea</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Norway</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>USA</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Germany</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Canada</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -1731,10 +1779,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$E$57:$E$73</c:f>
+              <c:f>'Calculos COVID19'!$E$62:$E$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>113</c:v>
                 </c:pt>
@@ -1760,13 +1808,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
@@ -1781,9 +1829,12 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3090,13 +3141,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3126,13 +3177,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3458,10 +3509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3BD7B-3B40-A94B-99F4-AAD0A2BEB996}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O65" sqref="O65"/>
+    <sheetView tabSelected="1" topLeftCell="D56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3539,11 +3590,11 @@
         <v>60.48</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F18" si="0">B3/E3</f>
+        <f t="shared" ref="F3:F19" si="0">B3/E3</f>
         <v>1143.7830687830688</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G18" si="1">D3/E3</f>
+        <f t="shared" ref="G3:G19" si="1">D3/E3</f>
         <v>112.76455026455027</v>
       </c>
       <c r="H3" s="2"/>
@@ -3949,630 +4000,725 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E19" s="4"/>
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1591</v>
+      </c>
+      <c r="C19" s="2">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2">
+        <v>32</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5.6</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="0"/>
+        <v>284.10714285714289</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="1"/>
+        <v>5.7142857142857144</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="5">
-        <v>800.81680280046669</v>
-      </c>
-      <c r="C22" s="5">
-        <v>872.11201866977831</v>
-      </c>
-      <c r="D22">
-        <v>997</v>
-      </c>
-      <c r="E22">
-        <v>1153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="5">
-        <v>885.87962962962968</v>
-      </c>
-      <c r="C23" s="5">
-        <v>977.81084656084658</v>
-      </c>
-      <c r="D23">
-        <v>1057</v>
-      </c>
-      <c r="E23" s="5">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="5">
-        <v>546.42091727389629</v>
-      </c>
-      <c r="C24" s="5">
-        <v>613.00900128589808</v>
-      </c>
-      <c r="D24">
-        <v>709</v>
-      </c>
-      <c r="E24">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="5">
-        <v>339.22902494331066</v>
-      </c>
-      <c r="C25" s="5">
-        <v>405.89569160997729</v>
-      </c>
-      <c r="D25">
-        <v>507</v>
-      </c>
-      <c r="E25">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="5">
-        <v>403.12965722801783</v>
-      </c>
-      <c r="C26" s="5">
-        <v>421.5722801788375</v>
-      </c>
-      <c r="D26">
-        <v>474</v>
-      </c>
-      <c r="E26">
-        <v>518</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B27" s="5">
-        <v>270.12924266215725</v>
+        <v>800.81680280046669</v>
       </c>
       <c r="C27" s="5">
-        <v>300</v>
+        <v>872.11201866977831</v>
       </c>
       <c r="D27">
-        <v>351</v>
+        <v>997</v>
       </c>
       <c r="E27">
-        <v>398</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B28" s="5">
-        <v>246.92982456140351</v>
+        <v>885.87962962962968</v>
       </c>
       <c r="C28" s="5">
-        <v>298</v>
+        <v>977.81084656084658</v>
       </c>
       <c r="D28">
-        <v>328</v>
-      </c>
-      <c r="E28">
-        <v>374</v>
+        <v>1057</v>
+      </c>
+      <c r="E28" s="5">
+        <v>1144</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B29" s="5">
-        <v>215.83818480370206</v>
+        <v>546.42091727389629</v>
       </c>
       <c r="C29" s="5">
-        <v>239</v>
+        <v>613.00900128589808</v>
       </c>
       <c r="D29">
-        <v>296</v>
+        <v>709</v>
       </c>
       <c r="E29">
-        <v>333</v>
+        <v>855</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" s="5">
-        <v>211.35040745052387</v>
+        <v>339.22902494331066</v>
       </c>
       <c r="C30" s="5">
-        <v>245</v>
+        <v>405.89569160997729</v>
       </c>
       <c r="D30">
-        <v>276</v>
+        <v>507</v>
       </c>
       <c r="E30">
-        <v>324</v>
+        <v>599</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B31" s="5">
-        <v>253.94282897979301</v>
+        <v>403.12965722801783</v>
       </c>
       <c r="C31" s="5">
-        <v>267</v>
+        <v>421.5722801788375</v>
       </c>
       <c r="D31">
-        <v>284</v>
+        <v>474</v>
       </c>
       <c r="E31">
-        <v>306</v>
+        <v>518</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B32" s="5">
-        <v>174.901185770751</v>
+        <v>270.12924266215725</v>
       </c>
       <c r="C32" s="5">
-        <v>191</v>
+        <v>300</v>
       </c>
       <c r="D32">
-        <v>202</v>
+        <v>351</v>
       </c>
       <c r="E32">
-        <v>226</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B33" s="5">
-        <v>170.95395375947155</v>
+        <v>246.92982456140351</v>
       </c>
       <c r="C33" s="5">
-        <v>173</v>
+        <v>298</v>
       </c>
       <c r="D33">
-        <v>174</v>
+        <v>328</v>
       </c>
       <c r="E33">
-        <v>176</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B34" s="5">
-        <v>73.67053789731051</v>
+        <v>215.83818480370206</v>
       </c>
       <c r="C34" s="5">
-        <v>99</v>
+        <v>239</v>
       </c>
       <c r="D34">
-        <v>129</v>
+        <v>296</v>
       </c>
       <c r="E34">
-        <v>162</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B35" s="5">
-        <v>75.526791089705</v>
+        <v>211.35040745052387</v>
       </c>
       <c r="C35" s="5">
-        <v>86</v>
+        <v>245</v>
       </c>
       <c r="D35">
-        <v>100</v>
+        <v>276</v>
       </c>
       <c r="E35">
-        <v>122</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B36" s="5">
-        <v>35.328544825751528</v>
+        <v>253.94282897979301</v>
       </c>
       <c r="C36" s="5">
-        <v>38</v>
+        <v>267</v>
       </c>
       <c r="D36">
-        <v>54</v>
+        <v>284</v>
       </c>
       <c r="E36">
-        <v>69</v>
+        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B37" s="5">
-        <v>58.447330447330444</v>
+        <v>251</v>
       </c>
       <c r="C37" s="5">
-        <v>58</v>
-      </c>
-      <c r="D37" s="5">
-        <v>59</v>
-      </c>
-      <c r="E37" s="5">
-        <v>59</v>
+        <v>262</v>
+      </c>
+      <c r="D37">
+        <v>282</v>
+      </c>
+      <c r="E37">
+        <v>284</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="5">
+        <v>174.901185770751</v>
+      </c>
+      <c r="C38" s="5">
+        <v>191</v>
+      </c>
+      <c r="D38">
+        <v>202</v>
+      </c>
+      <c r="E38">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="5">
+        <v>170.95395375947155</v>
+      </c>
+      <c r="C39" s="5">
+        <v>173</v>
+      </c>
+      <c r="D39">
+        <v>174</v>
+      </c>
+      <c r="E39">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="5">
+        <v>73.67053789731051</v>
+      </c>
+      <c r="C40" s="5">
+        <v>99</v>
+      </c>
+      <c r="D40">
+        <v>129</v>
+      </c>
+      <c r="E40">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="5">
+        <v>75.526791089705</v>
+      </c>
+      <c r="C41" s="5">
+        <v>86</v>
+      </c>
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="5">
+        <v>35.328544825751528</v>
+      </c>
+      <c r="C42" s="5">
+        <v>38</v>
+      </c>
+      <c r="D42">
+        <v>54</v>
+      </c>
+      <c r="E42">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="5">
+        <v>58.447330447330444</v>
+      </c>
+      <c r="C43" s="5">
+        <v>58</v>
+      </c>
+      <c r="D43" s="5">
+        <v>59</v>
+      </c>
+      <c r="E43" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B44" s="5">
         <v>3.9942938659058487</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C44" s="5">
         <v>5</v>
       </c>
-      <c r="D38">
+      <c r="D44">
         <v>6</v>
       </c>
-      <c r="E38">
+      <c r="E44">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>13</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D61" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E61" s="7" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" s="5">
-        <v>79.778439153439152</v>
-      </c>
-      <c r="C57" s="6">
-        <v>90.542328042328052</v>
-      </c>
-      <c r="D57">
-        <v>100</v>
-      </c>
-      <c r="E57">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B58" s="5">
-        <v>29.532790398628379</v>
-      </c>
-      <c r="C58" s="6">
-        <v>37.633947706815263</v>
-      </c>
-      <c r="D58">
-        <v>47</v>
-      </c>
-      <c r="E58">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" s="5">
-        <v>19.172005914243471</v>
-      </c>
-      <c r="C59">
-        <v>21</v>
-      </c>
-      <c r="D59">
-        <v>22</v>
-      </c>
-      <c r="E59">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B60" s="5">
-        <v>8.3893118375876998</v>
-      </c>
-      <c r="C60">
-        <v>10</v>
-      </c>
-      <c r="D60">
-        <v>13</v>
-      </c>
-      <c r="E60">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B61" s="5">
-        <v>7.9161816065192081</v>
-      </c>
-      <c r="C61">
-        <v>10</v>
-      </c>
-      <c r="D61">
-        <v>12</v>
-      </c>
-      <c r="E61">
-        <v>16</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B62" s="5">
-        <v>9.3348891481913654</v>
-      </c>
-      <c r="C62">
-        <v>11</v>
+        <v>79.778439153439152</v>
+      </c>
+      <c r="C62" s="6">
+        <v>90.542328042328052</v>
       </c>
       <c r="D62">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="E62">
-        <v>14</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B63" s="5">
-        <v>5.8771929824561404</v>
-      </c>
-      <c r="C63">
-        <v>7</v>
+        <v>29.532790398628379</v>
+      </c>
+      <c r="C63" s="6">
+        <v>37.633947706815263</v>
       </c>
       <c r="D63">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="E63">
-        <v>11</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B64" s="5">
-        <v>3.5069235400361229</v>
+        <v>19.172005914243471</v>
       </c>
       <c r="C64">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D64">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E64">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B65" s="5">
-        <v>1.9762845849802373</v>
+        <v>8.3893118375876998</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B66" s="5">
-        <v>0.90702947845804982</v>
+        <v>7.9161816065192081</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E66">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B67" s="5">
-        <v>2.3484848484848486</v>
+        <v>9.3348891481913654</v>
       </c>
       <c r="C67">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E67">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="5">
+        <v>5.8771929824561404</v>
+      </c>
+      <c r="C68">
         <v>7</v>
       </c>
-      <c r="B68" s="5">
-        <v>1.9817369341363902</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
       <c r="D68">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E68">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B69" s="5">
-        <v>1.3040238450074515</v>
+        <v>3.5069235400361229</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="5">
         <v>3</v>
       </c>
-      <c r="B70" s="5">
-        <v>0.91992665036674814</v>
-      </c>
       <c r="C70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E70">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" s="5">
+        <v>1.9762845849802373</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
         <v>4</v>
-      </c>
-      <c r="B71" s="5">
-        <v>1.0146152917018962</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71">
-        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B72" s="5">
-        <v>0.50545357807927638</v>
+        <v>0.90702947845804982</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="5">
+        <v>2.3484848484848486</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="5">
+        <v>1.9817369341363902</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75" s="5">
+        <v>1.3040238450074515</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="5">
+        <v>0.91992665036674814</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77" s="5">
+        <v>1.0146152917018962</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" s="5">
+        <v>0.50545357807927638</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B79" s="5">
         <v>0</v>
       </c>
-      <c r="C73">
+      <c r="C79">
         <v>0</v>
       </c>
-      <c r="D73">
+      <c r="D79">
         <v>0</v>
       </c>
-      <c r="E73">
+      <c r="E79">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A57:E73">
-    <sortCondition descending="1" ref="E57:E73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:E79">
+    <sortCondition descending="1" ref="E62:E79"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B25:C25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1C6950EC-FAC0-9C45-A0E5-F322505E906D}"/>
@@ -4591,38 +4737,38 @@
     <hyperlink ref="A15" r:id="rId14" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{EFD81247-2449-C842-A355-C3CA98069F0C}"/>
     <hyperlink ref="A16" r:id="rId15" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{6A5FA689-4530-FC48-8476-8EB82E5F1FB4}"/>
     <hyperlink ref="A17" r:id="rId16" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{768069AF-3C8F-EA44-BDE0-CFAD42D2AE89}"/>
-    <hyperlink ref="A37" r:id="rId17" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{2749059A-A8E1-B840-90D7-560A71410172}"/>
-    <hyperlink ref="A23" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
-    <hyperlink ref="A24" r:id="rId19" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{57A3EA1C-224C-3F47-BBF4-F96842A83158}"/>
-    <hyperlink ref="A34" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
-    <hyperlink ref="A27" r:id="rId21" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{AB6442DB-502D-BF47-BD97-FD78208EA473}"/>
-    <hyperlink ref="A31" r:id="rId22" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{E8933148-C5A5-C049-998E-8A19BCC472EE}"/>
-    <hyperlink ref="A29" r:id="rId23" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{148898F7-DFEC-AD49-AE18-589CAE84737B}"/>
-    <hyperlink ref="A33" r:id="rId24" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{C028FE55-7852-3F41-9817-549C985F7260}"/>
-    <hyperlink ref="A22" r:id="rId25" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{B5BDCE1C-B9BF-5D4E-AF41-63D149E1115B}"/>
-    <hyperlink ref="A35" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
-    <hyperlink ref="A30" r:id="rId27" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{D6541E56-79D1-DD4C-89C0-B9FE943CF17D}"/>
-    <hyperlink ref="A25" r:id="rId28" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{DB82E052-EA56-4542-B5D9-CDCA3F75C63F}"/>
-    <hyperlink ref="A28" r:id="rId29" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{B76E0484-5117-5040-B058-D17B21DC5420}"/>
-    <hyperlink ref="A26" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
-    <hyperlink ref="A32" r:id="rId31" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{219CBCE6-9D2C-5146-B0CA-29FE2A0FA513}"/>
-    <hyperlink ref="A36" r:id="rId32" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{A66187B1-4AD9-444B-BCFA-FF8464EDFF33}"/>
-    <hyperlink ref="A67" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
-    <hyperlink ref="A57" r:id="rId34" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{A20FB0CD-F9DA-914E-B2F5-F280E65964E3}"/>
-    <hyperlink ref="A58" r:id="rId35" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{EE62FA68-128F-064D-A4F8-F9BE8B79FC59}"/>
-    <hyperlink ref="A70" r:id="rId36" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{D2FB73FA-EC57-274E-BF29-C09B1AC3DDE2}"/>
-    <hyperlink ref="A71" r:id="rId37" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{523B8969-55CC-FF4F-9FA9-106BC6D662B5}"/>
-    <hyperlink ref="A59" r:id="rId38" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{517487C3-ADE3-274F-9F6E-78AC36F61827}"/>
-    <hyperlink ref="A60" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
-    <hyperlink ref="A68" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
-    <hyperlink ref="A62" r:id="rId41" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{92D1F4A4-B981-3C45-A55A-E63BE05C7D4F}"/>
-    <hyperlink ref="A64" r:id="rId42" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{9E857743-3BA1-D547-A532-A53EF891F862}"/>
-    <hyperlink ref="A61" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
-    <hyperlink ref="A66" r:id="rId44" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{76C0B263-3E56-DD44-BF90-D7A725F4C11B}"/>
-    <hyperlink ref="A63" r:id="rId45" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{F788A2F0-F76C-0A46-84F6-32311CDCE6EB}"/>
-    <hyperlink ref="A69" r:id="rId46" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{1FA4FB2B-21FB-A240-B716-855DE4CC3FCA}"/>
-    <hyperlink ref="A65" r:id="rId47" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{52773F30-B0DE-FE41-B798-80BFDD6B52F9}"/>
-    <hyperlink ref="A72" r:id="rId48" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{03FEC42E-DDC8-9B40-8CF7-F008D15BED91}"/>
+    <hyperlink ref="A43" r:id="rId17" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{2749059A-A8E1-B840-90D7-560A71410172}"/>
+    <hyperlink ref="A28" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
+    <hyperlink ref="A29" r:id="rId19" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{57A3EA1C-224C-3F47-BBF4-F96842A83158}"/>
+    <hyperlink ref="A40" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
+    <hyperlink ref="A32" r:id="rId21" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{AB6442DB-502D-BF47-BD97-FD78208EA473}"/>
+    <hyperlink ref="A36" r:id="rId22" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{E8933148-C5A5-C049-998E-8A19BCC472EE}"/>
+    <hyperlink ref="A34" r:id="rId23" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{148898F7-DFEC-AD49-AE18-589CAE84737B}"/>
+    <hyperlink ref="A39" r:id="rId24" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{C028FE55-7852-3F41-9817-549C985F7260}"/>
+    <hyperlink ref="A27" r:id="rId25" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{B5BDCE1C-B9BF-5D4E-AF41-63D149E1115B}"/>
+    <hyperlink ref="A41" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
+    <hyperlink ref="A35" r:id="rId27" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{D6541E56-79D1-DD4C-89C0-B9FE943CF17D}"/>
+    <hyperlink ref="A30" r:id="rId28" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{DB82E052-EA56-4542-B5D9-CDCA3F75C63F}"/>
+    <hyperlink ref="A33" r:id="rId29" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{B76E0484-5117-5040-B058-D17B21DC5420}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
+    <hyperlink ref="A38" r:id="rId31" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{219CBCE6-9D2C-5146-B0CA-29FE2A0FA513}"/>
+    <hyperlink ref="A42" r:id="rId32" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{A66187B1-4AD9-444B-BCFA-FF8464EDFF33}"/>
+    <hyperlink ref="A73" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
+    <hyperlink ref="A62" r:id="rId34" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{A20FB0CD-F9DA-914E-B2F5-F280E65964E3}"/>
+    <hyperlink ref="A63" r:id="rId35" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{EE62FA68-128F-064D-A4F8-F9BE8B79FC59}"/>
+    <hyperlink ref="A76" r:id="rId36" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{D2FB73FA-EC57-274E-BF29-C09B1AC3DDE2}"/>
+    <hyperlink ref="A77" r:id="rId37" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{523B8969-55CC-FF4F-9FA9-106BC6D662B5}"/>
+    <hyperlink ref="A64" r:id="rId38" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{517487C3-ADE3-274F-9F6E-78AC36F61827}"/>
+    <hyperlink ref="A65" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
+    <hyperlink ref="A74" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
+    <hyperlink ref="A67" r:id="rId41" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{92D1F4A4-B981-3C45-A55A-E63BE05C7D4F}"/>
+    <hyperlink ref="A69" r:id="rId42" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{9E857743-3BA1-D547-A532-A53EF891F862}"/>
+    <hyperlink ref="A66" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
+    <hyperlink ref="A72" r:id="rId44" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{76C0B263-3E56-DD44-BF90-D7A725F4C11B}"/>
+    <hyperlink ref="A68" r:id="rId45" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{F788A2F0-F76C-0A46-84F6-32311CDCE6EB}"/>
+    <hyperlink ref="A75" r:id="rId46" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{1FA4FB2B-21FB-A240-B716-855DE4CC3FCA}"/>
+    <hyperlink ref="A71" r:id="rId47" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{52773F30-B0DE-FE41-B798-80BFDD6B52F9}"/>
+    <hyperlink ref="A78" r:id="rId48" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{03FEC42E-DDC8-9B40-8CF7-F008D15BED91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId49"/>

</xml_diff>

<commit_message>
Update 25 MArch Brazil Added
</commit_message>
<xml_diff>
--- a/COVID19 calculos.xlsx
+++ b/COVID19 calculos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rramirez/projects/git-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA75E01-B8B3-2F49-A035-D6062D7BFB62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10028A0A-B9ED-B546-9AC2-3883203C8448}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="980" windowWidth="37020" windowHeight="17380" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
+    <workbookView xWindow="1220" yWindow="4020" windowWidth="37020" windowHeight="17380" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculos COVID19" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>China</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Denmark</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>25 March</t>
   </si>
 </sst>
 </file>
@@ -320,9 +326,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$45</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -360,13 +366,13 @@
                   <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>USA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Canada</c:v>
@@ -375,6 +381,9 @@
                   <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -382,10 +391,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$B$27:$B$44</c:f>
+              <c:f>'Calculos COVID19'!$B$27:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>800.81680280046669</c:v>
                 </c:pt>
@@ -423,13 +432,13 @@
                   <c:v>174.901185770751</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>73.67053789731051</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>75.526791089705</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>170.95395375947155</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>73.67053789731051</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75.526791089705</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>35.328544825751528</c:v>
@@ -438,6 +447,9 @@
                   <c:v>58.447330447330444</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>3.9942938659058487</c:v>
                 </c:pt>
               </c:numCache>
@@ -475,9 +487,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$45</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -515,13 +527,13 @@
                   <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>USA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Canada</c:v>
@@ -530,6 +542,9 @@
                   <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -537,10 +552,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$C$27:$C$44</c:f>
+              <c:f>'Calculos COVID19'!$C$27:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>872.11201866977831</c:v>
                 </c:pt>
@@ -578,13 +593,13 @@
                   <c:v>191</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>38</c:v>
@@ -593,6 +608,9 @@
                   <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -630,9 +648,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$45</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -670,13 +688,13 @@
                   <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>USA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Canada</c:v>
@@ -685,6 +703,9 @@
                   <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -692,10 +713,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$D$27:$D$44</c:f>
+              <c:f>'Calculos COVID19'!$D$27:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>997</c:v>
                 </c:pt>
@@ -733,13 +754,13 @@
                   <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>129</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>54</c:v>
@@ -748,6 +769,9 @@
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -785,9 +809,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$27:$A$44</c:f>
+              <c:f>'Calculos COVID19'!$A$27:$A$45</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Switzerland</c:v>
                 </c:pt>
@@ -825,13 +849,13 @@
                   <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>USA</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Canada</c:v>
@@ -840,6 +864,9 @@
                   <c:v>China</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Colombia</c:v>
                 </c:pt>
               </c:strCache>
@@ -847,10 +874,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$E$27:$E$44</c:f>
+              <c:f>'Calculos COVID19'!$E$27:$E$45</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>1153</c:v>
                 </c:pt>
@@ -888,13 +915,13 @@
                   <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
                   <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
                   <c:v>69</c:v>
@@ -903,6 +930,9 @@
                   <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
                   <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
@@ -911,6 +941,167 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E4A6-FA42-ADDC-2F07F0000D6D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$F$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>25 March</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$27:$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$F$27:$F$45</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>1272</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>634</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>451</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>377</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>373</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B266-AF46-828F-81A9D927F79A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1252,9 +1443,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$80</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1265,10 +1456,10 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Switzerland</c:v>
@@ -1289,16 +1480,16 @@
                   <c:v>Austria</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Germany</c:v>
@@ -1308,16 +1499,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Colombia</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Brazil</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$B$62:$B$79</c:f>
+              <c:f>'Calculos COVID19'!$B$62:$B$80</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>79.778439153439152</c:v>
                 </c:pt>
@@ -1328,10 +1522,10 @@
                   <c:v>19.172005914243471</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>7.9161816065192081</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8.3893118375876998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.9161816065192081</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>9.3348891481913654</c:v>
@@ -1352,16 +1546,16 @@
                   <c:v>0.90702947845804982</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1.3040238450074515</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91992665036674814</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2.3484848484848486</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>1.9817369341363902</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.3040238450074515</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.91992665036674814</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1.0146152917018962</c:v>
@@ -1370,6 +1564,9 @@
                   <c:v>0.50545357807927638</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1407,9 +1604,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$80</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1420,10 +1617,10 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Switzerland</c:v>
@@ -1444,16 +1641,16 @@
                   <c:v>Austria</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Germany</c:v>
@@ -1463,16 +1660,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Colombia</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Brazil</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$C$62:$C$79</c:f>
+              <c:f>'Calculos COVID19'!$C$62:$C$80</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>90.542328042328052</c:v>
                 </c:pt>
@@ -1507,16 +1707,16 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="14" formatCode="General">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
                   <c:v>1</c:v>
@@ -1525,6 +1725,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1562,9 +1765,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$80</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1575,10 +1778,10 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Switzerland</c:v>
@@ -1599,16 +1802,16 @@
                   <c:v>Austria</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Germany</c:v>
@@ -1618,16 +1821,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Colombia</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Brazil</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$D$62:$D$79</c:f>
+              <c:f>'Calculos COVID19'!$D$62:$D$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -1638,10 +1844,10 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14</c:v>
@@ -1680,6 +1886,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1717,9 +1926,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Calculos COVID19'!$A$62:$A$79</c:f>
+              <c:f>'Calculos COVID19'!$A$62:$A$80</c:f>
               <c:strCache>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Italy</c:v>
                 </c:pt>
@@ -1730,10 +1939,10 @@
                   <c:v>Iran</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>France</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Switzerland</c:v>
@@ -1754,16 +1963,16 @@
                   <c:v>Austria</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>China</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>S. Korea</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>Germany</c:v>
@@ -1773,16 +1982,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>Colombia</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Brazil</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Calculos COVID19'!$E$62:$E$79</c:f>
+              <c:f>'Calculos COVID19'!$E$62:$E$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>113</c:v>
                 </c:pt>
@@ -1835,6 +2047,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1843,6 +2058,167 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F899-1742-8A20-7614E15055DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$F$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>25 March</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$62:$A$80</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$F$62:$F$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E31A-2C4F-B261-46EB79EF9BB3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3139,16 +3515,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19627</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>175491</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>242454</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>175491</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3175,16 +3551,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>79663</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>115455</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>549563</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>115455</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3509,10 +3885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3BD7B-3B40-A94B-99F4-AAD0A2BEB996}">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D56" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3551,24 +3927,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>81171</v>
+        <v>81218</v>
       </c>
       <c r="C2" s="2">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2">
-        <v>3277</v>
+        <v>3281</v>
       </c>
       <c r="E2" s="3">
         <v>1386</v>
       </c>
       <c r="F2" s="5">
         <f>B2/E2</f>
-        <v>58.564935064935064</v>
+        <v>58.5988455988456</v>
       </c>
       <c r="G2" s="5">
         <f>D2/E2</f>
-        <v>2.3643578643578644</v>
+        <v>2.3672438672438672</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -3578,24 +3954,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>69176</v>
+        <v>74386</v>
       </c>
       <c r="C3" s="2">
-        <v>5249</v>
+        <v>5210</v>
       </c>
       <c r="D3" s="2">
-        <v>6820</v>
+        <v>7503</v>
       </c>
       <c r="E3" s="4">
         <v>60.48</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F19" si="0">B3/E3</f>
-        <v>1143.7830687830688</v>
+        <f t="shared" ref="F3:F20" si="0">B3/E3</f>
+        <v>1229.9272486772488</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G19" si="1">D3/E3</f>
-        <v>112.76455026455027</v>
+        <f t="shared" ref="G3:G20" si="1">D3/E3</f>
+        <v>124.05753968253968</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -3632,51 +4008,54 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>52983</v>
+        <v>64775</v>
       </c>
       <c r="C5" s="2">
-        <v>9249</v>
+        <v>9919</v>
       </c>
       <c r="D5" s="2">
-        <v>685</v>
+        <v>910</v>
       </c>
       <c r="E5" s="4">
         <v>327.2</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>161.92848410757946</v>
+        <v>197.96760391198043</v>
       </c>
       <c r="G5" s="5">
         <f>D5/E5</f>
-        <v>2.0935207823960882</v>
+        <v>2.7811735941320292</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2">
+        <f>E5*0.03</f>
+        <v>9.8159999999999989</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>32986</v>
+        <v>37323</v>
       </c>
       <c r="C6" s="2">
-        <v>3903</v>
+        <v>4332</v>
       </c>
       <c r="D6" s="2">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="E6" s="4">
         <v>82.79</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>398.42976204855654</v>
+        <v>450.81531585940326</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>1.8963642952047348</v>
+        <v>2.4882232153641741</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -3686,24 +4065,24 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>24811</v>
+        <v>27017</v>
       </c>
       <c r="C7" s="2">
-        <v>1762</v>
+        <v>2206</v>
       </c>
       <c r="D7" s="2">
-        <v>1934</v>
+        <v>2077</v>
       </c>
       <c r="E7" s="4">
         <v>81.16</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>305.70478068013801</v>
+        <v>332.88565795958601</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="1"/>
-        <v>23.829472646623955</v>
+        <v>25.59142434696895</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -3713,24 +4092,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>22304</v>
+        <v>25233</v>
       </c>
       <c r="C8" s="2">
-        <v>2448</v>
+        <v>2929</v>
       </c>
       <c r="D8" s="2">
-        <v>1100</v>
+        <v>1331</v>
       </c>
       <c r="E8" s="4">
         <v>66.989999999999995</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>332.94521570383642</v>
+        <v>376.66815942678016</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="1"/>
-        <v>16.420361247947454</v>
+        <v>19.868637110016422</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3740,24 +4119,24 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>9037</v>
+        <v>9137</v>
       </c>
       <c r="C9" s="2">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="D9" s="2">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E9" s="4">
         <v>51.47</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>175.5780066057898</v>
+        <v>177.52088595298233</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>2.3314552166310474</v>
+        <v>2.4480279774625995</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -3767,24 +4146,24 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>9877</v>
+        <v>10897</v>
       </c>
       <c r="C10" s="2">
-        <v>1082</v>
+        <v>1020</v>
       </c>
       <c r="D10" s="2">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="E10" s="4">
         <v>8.57</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>1152.5087514585764</v>
+        <v>1271.5285880980164</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>14.235705950991832</v>
+        <v>17.852975495915985</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3794,24 +4173,24 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>8077</v>
+        <v>9529</v>
       </c>
       <c r="C11" s="2">
-        <v>1427</v>
+        <v>1452</v>
       </c>
       <c r="D11" s="2">
-        <v>422</v>
+        <v>465</v>
       </c>
       <c r="E11" s="4">
         <v>66.44</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>121.56833232992174</v>
+        <v>143.42263696568332</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="1"/>
-        <v>6.351595424443107</v>
+        <v>6.9987959060806748</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3821,24 +4200,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>5560</v>
+        <v>6412</v>
       </c>
       <c r="C12" s="2">
-        <v>811</v>
+        <v>852</v>
       </c>
       <c r="D12" s="2">
-        <v>276</v>
+        <v>356</v>
       </c>
       <c r="E12" s="4">
         <v>17.18</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>323.63213038416762</v>
+        <v>373.22467986030267</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="1"/>
-        <v>16.065192083818395</v>
+        <v>20.721769499417928</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -3848,24 +4227,24 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>5283</v>
+        <v>5588</v>
       </c>
       <c r="C13" s="2">
-        <v>809</v>
+        <v>305</v>
       </c>
       <c r="D13" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E13" s="4">
         <v>8.82</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>598.9795918367347</v>
+        <v>633.56009070294783</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="1"/>
-        <v>3.1746031746031744</v>
+        <v>3.4013605442176869</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3875,24 +4254,24 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>4269</v>
+        <v>4937</v>
       </c>
       <c r="C14" s="2">
-        <v>526</v>
+        <v>668</v>
       </c>
       <c r="D14" s="2">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="E14" s="4">
         <v>11.4</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>374.4736842105263</v>
+        <v>433.07017543859649</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="1"/>
-        <v>10.701754385964913</v>
+        <v>15.614035087719298</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -3902,24 +4281,24 @@
         <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>2779</v>
+        <v>3066</v>
       </c>
       <c r="C15" s="2">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="D15" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E15" s="4">
         <v>5.3680000000000003</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="0"/>
-        <v>517.69746646795829</v>
+        <v>571.16244411326375</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="1"/>
-        <v>2.2354694485842024</v>
+        <v>2.608047690014903</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3927,24 +4306,24 @@
         <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>2286</v>
+        <v>2526</v>
       </c>
       <c r="C16" s="2">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="D16" s="2">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E16" s="4">
         <v>10.119999999999999</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>225.88932806324112</v>
+        <v>249.60474308300397</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="1"/>
-        <v>3.5573122529644272</v>
+        <v>6.1264822134387353</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3954,24 +4333,24 @@
         <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>2590</v>
+        <v>3306</v>
       </c>
       <c r="C17" s="2">
-        <v>499</v>
+        <v>514</v>
       </c>
       <c r="D17" s="2">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E17" s="4">
         <v>37.590000000000003</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>68.901303538175043</v>
+        <v>87.94892258579408</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="1"/>
-        <v>0.66507049747273206</v>
+        <v>0.79808459696727851</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -4004,43 +4383,73 @@
         <v>28</v>
       </c>
       <c r="B19" s="2">
-        <v>1591</v>
+        <v>1724</v>
       </c>
       <c r="C19" s="2">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="D19" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="4">
         <v>5.6</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="0"/>
-        <v>284.10714285714289</v>
+        <v>307.85714285714289</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" si="1"/>
-        <v>5.7142857142857144</v>
+        <v>6.0714285714285721</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2433</v>
+      </c>
+      <c r="C20" s="2">
+        <v>186</v>
+      </c>
+      <c r="D20" s="2">
+        <v>57</v>
+      </c>
+      <c r="E20" s="4">
+        <v>209.3</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="0"/>
+        <v>11.624462494027711</v>
+      </c>
+      <c r="G20" s="5">
+        <f>D20/E20</f>
+        <v>0.27233635929288103</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="B21" s="2">
+        <v>1178</v>
+      </c>
+      <c r="C21" s="2">
+        <v>186</v>
+      </c>
+      <c r="D21" s="2">
+        <v>25</v>
+      </c>
+      <c r="E21" s="4">
+        <v>209.3</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" ref="F21" si="2">B21/E21</f>
+        <v>5.6282847587195413</v>
+      </c>
+      <c r="G21" s="5">
+        <f>D21/E21</f>
+        <v>0.11944577161968466</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -4083,6 +4492,9 @@
       <c r="E26" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="F26" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -4100,6 +4512,9 @@
       <c r="E27">
         <v>1153</v>
       </c>
+      <c r="F27">
+        <v>1272</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -4117,6 +4532,9 @@
       <c r="E28" s="5">
         <v>1144</v>
       </c>
+      <c r="F28" s="5">
+        <v>1230</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -4134,6 +4552,9 @@
       <c r="E29">
         <v>855</v>
       </c>
+      <c r="F29">
+        <v>855</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -4151,6 +4572,9 @@
       <c r="E30">
         <v>599</v>
       </c>
+      <c r="F30">
+        <v>634</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -4168,6 +4592,9 @@
       <c r="E31">
         <v>518</v>
       </c>
+      <c r="F31">
+        <v>571</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -4185,8 +4612,11 @@
       <c r="E32">
         <v>398</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
@@ -4202,8 +4632,11 @@
       <c r="E33">
         <v>374</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -4219,8 +4652,11 @@
       <c r="E34">
         <v>333</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -4236,8 +4672,11 @@
       <c r="E35">
         <v>324</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -4253,8 +4692,11 @@
       <c r="E36">
         <v>306</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
@@ -4270,8 +4712,11 @@
       <c r="E37">
         <v>284</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -4287,59 +4732,71 @@
       <c r="E38">
         <v>226</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="5">
+        <v>73.67053789731051</v>
+      </c>
+      <c r="C39" s="5">
+        <v>99</v>
+      </c>
+      <c r="D39">
+        <v>129</v>
+      </c>
+      <c r="E39">
+        <v>162</v>
+      </c>
+      <c r="F39">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="5">
+        <v>75.526791089705</v>
+      </c>
+      <c r="C40" s="5">
+        <v>86</v>
+      </c>
+      <c r="D40">
+        <v>100</v>
+      </c>
+      <c r="E40">
+        <v>122</v>
+      </c>
+      <c r="F40">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B41" s="5">
         <v>170.95395375947155</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C41" s="5">
         <v>173</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>174</v>
       </c>
-      <c r="E39">
+      <c r="E41">
         <v>176</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="5">
-        <v>73.67053789731051</v>
-      </c>
-      <c r="C40" s="5">
-        <v>99</v>
-      </c>
-      <c r="D40">
-        <v>129</v>
-      </c>
-      <c r="E40">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="5">
-        <v>75.526791089705</v>
-      </c>
-      <c r="C41" s="5">
-        <v>86</v>
-      </c>
-      <c r="D41">
-        <v>100</v>
-      </c>
-      <c r="E41">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>21</v>
       </c>
@@ -4355,8 +4812,11 @@
       <c r="E42">
         <v>69</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -4372,25 +4832,51 @@
       <c r="E43" s="5">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="5">
+        <v>6</v>
+      </c>
+      <c r="C44" s="5">
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <v>9</v>
+      </c>
+      <c r="E44">
+        <v>11</v>
+      </c>
+      <c r="F44">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B45" s="5">
         <v>3.9942938659058487</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C45" s="5">
         <v>5</v>
       </c>
-      <c r="D44">
+      <c r="D45">
         <v>6</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -4406,8 +4892,11 @@
       <c r="E61" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>1</v>
       </c>
@@ -4423,8 +4912,11 @@
       <c r="E62">
         <v>113</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -4440,8 +4932,11 @@
       <c r="E63">
         <v>60</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
@@ -4457,42 +4952,51 @@
       <c r="E64">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B65" s="5">
-        <v>8.3893118375876998</v>
+        <v>7.9161816065192081</v>
       </c>
       <c r="C65">
         <v>10</v>
       </c>
       <c r="D65">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E65">
         <v>16</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B66" s="5">
-        <v>7.9161816065192081</v>
+        <v>8.3893118375876998</v>
       </c>
       <c r="C66">
         <v>10</v>
       </c>
       <c r="D66">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E66">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>8</v>
       </c>
@@ -4508,8 +5012,11 @@
       <c r="E67">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>12</v>
       </c>
@@ -4525,8 +5032,11 @@
       <c r="E68">
         <v>11</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>9</v>
       </c>
@@ -4542,8 +5052,11 @@
       <c r="E69">
         <v>6</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>28</v>
       </c>
@@ -4559,8 +5072,11 @@
       <c r="E70">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>20</v>
       </c>
@@ -4576,8 +5092,11 @@
       <c r="E71">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>11</v>
       </c>
@@ -4593,16 +5112,19 @@
       <c r="E72">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B73" s="5">
-        <v>2.3484848484848486</v>
+        <v>1.3040238450074515</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -4610,16 +5132,19 @@
       <c r="E73">
         <v>2</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B74" s="5">
-        <v>1.9817369341363902</v>
+        <v>0.91992665036674814</v>
       </c>
       <c r="C74">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -4627,16 +5152,19 @@
       <c r="E74">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B75" s="5">
-        <v>1.3040238450074515</v>
+        <v>2.3484848484848486</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -4644,16 +5172,19 @@
       <c r="E75">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B76" s="5">
-        <v>0.91992665036674814</v>
+        <v>1.9817369341363902</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -4661,8 +5192,11 @@
       <c r="E76">
         <v>2</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
@@ -4678,8 +5212,11 @@
       <c r="E77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>21</v>
       </c>
@@ -4695,8 +5232,11 @@
       <c r="E78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>22</v>
       </c>
@@ -4712,10 +5252,33 @@
       <c r="E79">
         <v>0</v>
       </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B80" s="5">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:E79">
-    <sortCondition descending="1" ref="E62:E79"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:F80">
+    <sortCondition descending="1" ref="F62:F80"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B25:C25"/>
@@ -4740,33 +5303,33 @@
     <hyperlink ref="A43" r:id="rId17" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{2749059A-A8E1-B840-90D7-560A71410172}"/>
     <hyperlink ref="A28" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
     <hyperlink ref="A29" r:id="rId19" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{57A3EA1C-224C-3F47-BBF4-F96842A83158}"/>
-    <hyperlink ref="A40" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
+    <hyperlink ref="A39" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
     <hyperlink ref="A32" r:id="rId21" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{AB6442DB-502D-BF47-BD97-FD78208EA473}"/>
     <hyperlink ref="A36" r:id="rId22" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{E8933148-C5A5-C049-998E-8A19BCC472EE}"/>
     <hyperlink ref="A34" r:id="rId23" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{148898F7-DFEC-AD49-AE18-589CAE84737B}"/>
-    <hyperlink ref="A39" r:id="rId24" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{C028FE55-7852-3F41-9817-549C985F7260}"/>
+    <hyperlink ref="A41" r:id="rId24" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{C028FE55-7852-3F41-9817-549C985F7260}"/>
     <hyperlink ref="A27" r:id="rId25" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{B5BDCE1C-B9BF-5D4E-AF41-63D149E1115B}"/>
-    <hyperlink ref="A41" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
+    <hyperlink ref="A40" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
     <hyperlink ref="A35" r:id="rId27" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{D6541E56-79D1-DD4C-89C0-B9FE943CF17D}"/>
     <hyperlink ref="A30" r:id="rId28" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{DB82E052-EA56-4542-B5D9-CDCA3F75C63F}"/>
     <hyperlink ref="A33" r:id="rId29" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{B76E0484-5117-5040-B058-D17B21DC5420}"/>
     <hyperlink ref="A31" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
     <hyperlink ref="A38" r:id="rId31" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{219CBCE6-9D2C-5146-B0CA-29FE2A0FA513}"/>
     <hyperlink ref="A42" r:id="rId32" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{A66187B1-4AD9-444B-BCFA-FF8464EDFF33}"/>
-    <hyperlink ref="A73" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
+    <hyperlink ref="A75" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
     <hyperlink ref="A62" r:id="rId34" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{A20FB0CD-F9DA-914E-B2F5-F280E65964E3}"/>
     <hyperlink ref="A63" r:id="rId35" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{EE62FA68-128F-064D-A4F8-F9BE8B79FC59}"/>
-    <hyperlink ref="A76" r:id="rId36" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{D2FB73FA-EC57-274E-BF29-C09B1AC3DDE2}"/>
+    <hyperlink ref="A74" r:id="rId36" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{D2FB73FA-EC57-274E-BF29-C09B1AC3DDE2}"/>
     <hyperlink ref="A77" r:id="rId37" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{523B8969-55CC-FF4F-9FA9-106BC6D662B5}"/>
     <hyperlink ref="A64" r:id="rId38" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{517487C3-ADE3-274F-9F6E-78AC36F61827}"/>
-    <hyperlink ref="A65" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
-    <hyperlink ref="A74" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
+    <hyperlink ref="A66" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
+    <hyperlink ref="A76" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
     <hyperlink ref="A67" r:id="rId41" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{92D1F4A4-B981-3C45-A55A-E63BE05C7D4F}"/>
     <hyperlink ref="A69" r:id="rId42" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{9E857743-3BA1-D547-A532-A53EF891F862}"/>
-    <hyperlink ref="A66" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
+    <hyperlink ref="A65" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
     <hyperlink ref="A72" r:id="rId44" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{76C0B263-3E56-DD44-BF90-D7A725F4C11B}"/>
     <hyperlink ref="A68" r:id="rId45" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{F788A2F0-F76C-0A46-84F6-32311CDCE6EB}"/>
-    <hyperlink ref="A75" r:id="rId46" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{1FA4FB2B-21FB-A240-B716-855DE4CC3FCA}"/>
+    <hyperlink ref="A73" r:id="rId46" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{1FA4FB2B-21FB-A240-B716-855DE4CC3FCA}"/>
     <hyperlink ref="A71" r:id="rId47" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{52773F30-B0DE-FE41-B798-80BFDD6B52F9}"/>
     <hyperlink ref="A78" r:id="rId48" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{03FEC42E-DDC8-9B40-8CF7-F008D15BED91}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
update 2 april II
</commit_message>
<xml_diff>
--- a/COVID19 calculos.xlsx
+++ b/COVID19 calculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rramirez/projects/git-demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A799B94C-23AD-9E4D-9555-3DFF1D963066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8C0115-614D-2E44-89F1-8EA8E15B967E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
   <si>
     <t>China</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>2 April</t>
+  </si>
+  <si>
+    <t>3 April</t>
   </si>
 </sst>
 </file>
@@ -6034,10 +6037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3BD7B-3B40-A94B-99F4-AAD0A2BEB996}">
-  <dimension ref="A1:N80"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K54" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7455,7 +7458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -7498,8 +7501,11 @@
       <c r="N61" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="O61" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>1</v>
       </c>
@@ -7543,7 +7549,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>2</v>
       </c>
@@ -7587,7 +7593,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Uodate 6 April II
</commit_message>
<xml_diff>
--- a/COVID19 calculos.xlsx
+++ b/COVID19 calculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rramirez/projects/COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40752CA-74CF-3C42-BA63-8C9DF44440D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE29DC62-1D29-F542-98E7-1C6B75BD2B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
   <si>
     <t>China</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>5 April</t>
+  </si>
+  <si>
+    <t>6 April</t>
   </si>
 </sst>
 </file>
@@ -400,22 +403,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -466,22 +469,22 @@
                   <c:v>270.12924266215725</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>403.12965722801783</c:v>
+                  <c:v>73.67053789731051</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>211.35040745052387</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>73.67053789731051</c:v>
+                  <c:v>403.12965722801783</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>75.526791089705</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>253.94282897979301</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>75.526791089705</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>174.901185770751</c:v>
@@ -561,22 +564,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -627,22 +630,22 @@
                   <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>421.5722801788375</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>421.5722801788375</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>262</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>267</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>191</c:v>
@@ -722,22 +725,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -788,22 +791,22 @@
                   <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>474</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>129</c:v>
+                  <c:v>474</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>282</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>284</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>202</c:v>
@@ -883,22 +886,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -949,22 +952,22 @@
                   <c:v>398</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>518</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>162</c:v>
+                  <c:v>518</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>226</c:v>
@@ -1044,22 +1047,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -1110,22 +1113,22 @@
                   <c:v>451</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>571</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>198</c:v>
+                  <c:v>571</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>308</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>333</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>250</c:v>
@@ -1205,22 +1208,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -1271,22 +1274,22 @@
                   <c:v>531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>628</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>433</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>260</c:v>
+                  <c:v>628</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>362</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>281</c:v>
@@ -1368,22 +1371,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -1434,22 +1437,22 @@
                   <c:v>614</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>628</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>501</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>310</c:v>
+                  <c:v>628</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>365</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>398</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>371</c:v>
@@ -1531,22 +1534,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -1597,22 +1600,22 @@
                   <c:v>697</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>748</c:v>
+                  <c:v>369</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>568</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>369</c:v>
+                  <c:v>748</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>436</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>341</c:v>
@@ -1694,22 +1697,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -1760,22 +1763,22 @@
                   <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>758</c:v>
+                  <c:v>434</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>434</c:v>
+                  <c:v>758</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>428</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>472</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>366</c:v>
@@ -1857,22 +1860,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -1923,22 +1926,22 @@
                   <c:v>828</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>828</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>624</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>500</c:v>
+                  <c:v>828</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>511</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>333</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>398</c:v>
@@ -2020,22 +2023,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -2086,22 +2089,22 @@
                   <c:v>867</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>865</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>733</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>576</c:v>
+                  <c:v>865</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>511</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>550</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>438</c:v>
@@ -2183,22 +2186,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -2249,22 +2252,22 @@
                   <c:v>942</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>909</c:v>
+                  <c:v>658</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>792</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>658</c:v>
+                  <c:v>909</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>555</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>586</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>444</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>489</c:v>
@@ -2347,22 +2350,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -2413,22 +2416,22 @@
                   <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>959</c:v>
+                  <c:v>749</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>855</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>749</c:v>
+                  <c:v>959</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>605</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>622</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>507</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>550</c:v>
@@ -2511,22 +2514,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -2577,22 +2580,22 @@
                   <c:v>1101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1000</c:v>
+                  <c:v>847</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>915</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>847</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>655</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>574</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>606</c:v>
@@ -2675,22 +2678,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -2741,22 +2744,22 @@
                   <c:v>1161</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1034</c:v>
+                  <c:v>952</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>952</c:v>
+                  <c:v>1034</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>728</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>687</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>631</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>637</c:v>
@@ -2839,22 +2842,22 @@
                   <c:v>Germany</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Norway</c:v>
+                  <c:v>USA</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>USA</c:v>
+                  <c:v>Norway</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Denmark</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>Sweden</c:v>
@@ -2905,22 +2908,22 @@
                   <c:v>1209</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1059</c:v>
+                  <c:v>1029</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1039</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1029</c:v>
+                  <c:v>1059</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>780</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>745</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>675</c:v>
@@ -2946,6 +2949,170 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A4F2-1D4B-805D-75838CA8D2D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$R$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6 April</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$27:$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$R$27:$R$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>2929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2527</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0">
+                  <c:v>2192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1826</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1463</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1394</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1123</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1094</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1093</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>836</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-58D3-AE4C-AC9C-7A2DB6E006B4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3312,10 +3479,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -3339,10 +3506,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -3378,10 +3545,10 @@
                   <c:v>3.5069235400361229</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1.9762845849802373</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>19.172005914243471</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.9762845849802373</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3</c:v>
@@ -3405,10 +3572,10 @@
                   <c:v>1.9817369341363902</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2.3484848484848486</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -3473,10 +3640,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -3500,10 +3667,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -3539,10 +3706,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
                   <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
                   <c:v>4</c:v>
@@ -3566,10 +3733,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="General">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
                   <c:v>0</c:v>
@@ -3634,10 +3801,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -3661,10 +3828,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -3700,10 +3867,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4</c:v>
@@ -3727,10 +3894,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -3795,10 +3962,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -3822,10 +3989,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -3861,10 +4028,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>6</c:v>
@@ -3888,10 +4055,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -3956,10 +4123,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -3983,10 +4150,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -4022,10 +4189,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>6</c:v>
@@ -4049,10 +4216,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -4117,10 +4284,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -4144,10 +4311,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -4183,10 +4350,10 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7</c:v>
@@ -4210,10 +4377,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -4280,10 +4447,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -4307,10 +4474,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -4346,10 +4513,10 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9</c:v>
@@ -4373,10 +4540,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -4443,10 +4610,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -4470,10 +4637,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -4509,10 +4676,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>12</c:v>
@@ -4536,10 +4703,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -4606,10 +4773,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -4633,10 +4800,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -4672,10 +4839,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>13</c:v>
@@ -4699,10 +4866,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -4769,10 +4936,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -4796,10 +4963,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -4835,10 +5002,10 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>14</c:v>
@@ -4862,10 +5029,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -4932,10 +5099,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -4959,10 +5126,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -4998,10 +5165,10 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>16</c:v>
@@ -5025,10 +5192,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -5095,10 +5262,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -5122,10 +5289,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -5161,10 +5328,10 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>19</c:v>
@@ -5188,10 +5355,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -5259,10 +5426,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -5286,10 +5453,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -5325,10 +5492,10 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>22</c:v>
@@ -5423,10 +5590,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -5450,10 +5617,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -5489,10 +5656,10 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>25</c:v>
@@ -5587,10 +5754,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -5614,10 +5781,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -5653,10 +5820,10 @@
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>29</c:v>
@@ -5751,10 +5918,10 @@
                   <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Iran</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Sweden</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Denmark</c:v>
@@ -5778,10 +5945,10 @@
                   <c:v>S. Korea</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>China</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Brazil</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>Colombia</c:v>
@@ -5817,10 +5984,10 @@
                   <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>32</c:v>
@@ -5858,6 +6025,170 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F9A-6044-8D24-42FC698CD13B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$R$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6 April</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$62:$A$80</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$R$62:$R$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C6F-7346-A3B7-696B797AA1E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7526,8 +7857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3BD7B-3B40-A94B-99F4-AAD0A2BEB996}">
   <dimension ref="A1:AR80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="O52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AG34" sqref="AG34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7946,7 +8277,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
@@ -7969,7 +8300,7 @@
         <v>8.5927108273476982</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
         <v>22</v>
       </c>
@@ -7992,7 +8323,7 @@
         <v>0.93743631546769923</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
@@ -8015,7 +8346,7 @@
         <v>33.392857142857146</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>29</v>
       </c>
@@ -8040,7 +8371,7 @@
         <v>2.7042522694696607</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -8049,7 +8380,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -8058,7 +8389,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -8067,14 +8398,14 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -8126,8 +8457,11 @@
       <c r="Q26" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="R26" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -8179,8 +8513,11 @@
       <c r="Q27">
         <v>2821</v>
       </c>
+      <c r="R27">
+        <v>2929</v>
+      </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -8232,8 +8569,11 @@
       <c r="Q28">
         <v>2483</v>
       </c>
+      <c r="R28">
+        <v>2527</v>
+      </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -8285,8 +8625,11 @@
       <c r="Q29" s="5">
         <v>2132</v>
       </c>
+      <c r="R29" s="5">
+        <v>2192</v>
+      </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -8338,8 +8681,11 @@
       <c r="Q30">
         <v>1826</v>
       </c>
+      <c r="R30">
+        <v>1826</v>
+      </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -8391,8 +8737,11 @@
       <c r="Q31">
         <v>1386</v>
       </c>
+      <c r="R31">
+        <v>1463</v>
+      </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -8444,8 +8793,11 @@
       <c r="Q32">
         <v>1366</v>
       </c>
+      <c r="R32">
+        <v>1394</v>
+      </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -8497,61 +8849,67 @@
       <c r="Q33">
         <v>1209</v>
       </c>
+      <c r="R33">
+        <v>1249</v>
+      </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B34" s="5">
-        <v>403.12965722801783</v>
+        <v>73.67053789731051</v>
       </c>
       <c r="C34" s="5">
-        <v>421.5722801788375</v>
+        <v>99</v>
       </c>
       <c r="D34">
-        <v>474</v>
+        <v>129</v>
       </c>
       <c r="E34">
-        <v>518</v>
+        <v>162</v>
       </c>
       <c r="F34">
-        <v>571</v>
+        <v>198</v>
       </c>
       <c r="G34">
-        <v>628</v>
+        <v>260</v>
       </c>
       <c r="H34">
-        <v>628</v>
+        <v>310</v>
       </c>
       <c r="I34">
-        <v>748</v>
+        <v>369</v>
       </c>
       <c r="J34">
-        <v>758</v>
+        <v>434</v>
       </c>
       <c r="K34">
-        <v>828</v>
+        <v>500</v>
       </c>
       <c r="L34">
-        <v>865</v>
+        <v>576</v>
       </c>
       <c r="M34">
-        <v>909</v>
+        <v>658</v>
       </c>
       <c r="N34">
-        <v>959</v>
+        <v>749</v>
       </c>
       <c r="O34">
-        <v>1000</v>
+        <v>847</v>
       </c>
       <c r="P34">
-        <v>1034</v>
+        <v>952</v>
       </c>
       <c r="Q34">
-        <v>1059</v>
+        <v>1029</v>
+      </c>
+      <c r="R34">
+        <v>1123</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -8603,61 +8961,67 @@
       <c r="Q35">
         <v>1039</v>
       </c>
+      <c r="R35">
+        <v>1094</v>
+      </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B36" s="5">
-        <v>73.67053789731051</v>
+        <v>403.12965722801783</v>
       </c>
       <c r="C36" s="5">
-        <v>99</v>
+        <v>421.5722801788375</v>
       </c>
       <c r="D36">
-        <v>129</v>
+        <v>474</v>
       </c>
       <c r="E36">
-        <v>162</v>
+        <v>518</v>
       </c>
       <c r="F36">
-        <v>198</v>
+        <v>571</v>
       </c>
       <c r="G36">
-        <v>260</v>
+        <v>628</v>
       </c>
       <c r="H36">
-        <v>310</v>
+        <v>628</v>
       </c>
       <c r="I36">
-        <v>369</v>
+        <v>748</v>
       </c>
       <c r="J36">
-        <v>434</v>
+        <v>758</v>
       </c>
       <c r="K36">
-        <v>500</v>
+        <v>828</v>
       </c>
       <c r="L36">
-        <v>576</v>
+        <v>865</v>
       </c>
       <c r="M36">
-        <v>658</v>
+        <v>909</v>
       </c>
       <c r="N36">
-        <v>749</v>
+        <v>959</v>
       </c>
       <c r="O36">
-        <v>847</v>
+        <v>1000</v>
       </c>
       <c r="P36">
-        <v>952</v>
+        <v>1034</v>
       </c>
       <c r="Q36">
-        <v>1029</v>
+        <v>1059</v>
+      </c>
+      <c r="R36">
+        <v>1093</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
@@ -8709,114 +9073,123 @@
       <c r="Q37">
         <v>780</v>
       </c>
+      <c r="R37">
+        <v>836</v>
+      </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="5">
+        <v>75.526791089705</v>
+      </c>
+      <c r="C38" s="5">
+        <v>86</v>
+      </c>
+      <c r="D38">
+        <v>100</v>
+      </c>
+      <c r="E38">
+        <v>122</v>
+      </c>
+      <c r="F38">
+        <v>198</v>
+      </c>
+      <c r="G38">
+        <v>175</v>
+      </c>
+      <c r="H38">
+        <v>219</v>
+      </c>
+      <c r="I38">
+        <v>257</v>
+      </c>
+      <c r="J38">
+        <v>294</v>
+      </c>
+      <c r="K38">
+        <v>333</v>
+      </c>
+      <c r="L38">
+        <v>379</v>
+      </c>
+      <c r="M38">
+        <v>444</v>
+      </c>
+      <c r="N38">
+        <v>507</v>
+      </c>
+      <c r="O38">
+        <v>574</v>
+      </c>
+      <c r="P38">
+        <v>631</v>
+      </c>
+      <c r="Q38">
+        <v>720</v>
+      </c>
+      <c r="R38">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B39" s="5">
         <v>253.94282897979301</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>267</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>284</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>306</v>
       </c>
-      <c r="F38">
+      <c r="F39">
         <v>333</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <v>362</v>
       </c>
-      <c r="H38">
+      <c r="H39">
         <v>398</v>
       </c>
-      <c r="I38">
+      <c r="I39">
         <v>436</v>
       </c>
-      <c r="J38">
+      <c r="J39">
         <v>472</v>
       </c>
-      <c r="K38">
+      <c r="K39">
         <v>511</v>
       </c>
-      <c r="L38">
+      <c r="L39">
         <v>550</v>
       </c>
-      <c r="M38">
+      <c r="M39">
         <v>586</v>
       </c>
-      <c r="N38">
+      <c r="N39">
         <v>622</v>
       </c>
-      <c r="O38">
+      <c r="O39">
         <v>655</v>
       </c>
-      <c r="P38">
+      <c r="P39">
         <v>687</v>
       </c>
-      <c r="Q38">
+      <c r="Q39">
         <v>745</v>
       </c>
+      <c r="R39">
+        <v>745</v>
+      </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="5">
-        <v>75.526791089705</v>
-      </c>
-      <c r="C39" s="5">
-        <v>86</v>
-      </c>
-      <c r="D39">
-        <v>100</v>
-      </c>
-      <c r="E39">
-        <v>122</v>
-      </c>
-      <c r="F39">
-        <v>198</v>
-      </c>
-      <c r="G39">
-        <v>175</v>
-      </c>
-      <c r="H39">
-        <v>219</v>
-      </c>
-      <c r="I39">
-        <v>257</v>
-      </c>
-      <c r="J39">
-        <v>294</v>
-      </c>
-      <c r="K39">
-        <v>333</v>
-      </c>
-      <c r="L39">
-        <v>379</v>
-      </c>
-      <c r="M39">
-        <v>444</v>
-      </c>
-      <c r="N39">
-        <v>507</v>
-      </c>
-      <c r="O39">
-        <v>574</v>
-      </c>
-      <c r="P39">
-        <v>631</v>
-      </c>
-      <c r="Q39">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>20</v>
       </c>
@@ -8868,8 +9241,11 @@
       <c r="Q40">
         <v>675</v>
       </c>
+      <c r="R40">
+        <v>712</v>
+      </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -8921,8 +9297,11 @@
       <c r="Q41">
         <v>413</v>
       </c>
+      <c r="R41">
+        <v>443</v>
+      </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -8974,8 +9353,11 @@
       <c r="Q42">
         <v>199</v>
       </c>
+      <c r="R42">
+        <v>201</v>
+      </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>0</v>
       </c>
@@ -9027,8 +9409,11 @@
       <c r="Q43" s="5">
         <v>59</v>
       </c>
+      <c r="R43" s="5">
+        <v>59</v>
+      </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
@@ -9080,8 +9465,11 @@
       <c r="Q44">
         <v>54</v>
       </c>
+      <c r="R44">
+        <v>58</v>
+      </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
@@ -9133,8 +9521,11 @@
       <c r="Q45">
         <v>30</v>
       </c>
+      <c r="R45">
+        <v>32</v>
+      </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -9186,8 +9577,11 @@
       <c r="Q61" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="R61" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
@@ -9239,8 +9633,11 @@
       <c r="Q62">
         <v>271</v>
       </c>
+      <c r="R62">
+        <v>286</v>
+      </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
@@ -9292,8 +9689,11 @@
       <c r="Q63">
         <v>263</v>
       </c>
+      <c r="R63">
+        <v>273</v>
+      </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>12</v>
       </c>
@@ -9343,6 +9743,9 @@
         <v>113</v>
       </c>
       <c r="Q64">
+        <v>143</v>
+      </c>
+      <c r="R64">
         <v>143</v>
       </c>
     </row>
@@ -9398,6 +9801,9 @@
       <c r="Q65">
         <v>121</v>
       </c>
+      <c r="R65">
+        <v>133</v>
+      </c>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
@@ -9451,6 +9857,9 @@
       <c r="Q66">
         <v>103</v>
       </c>
+      <c r="R66">
+        <v>109</v>
+      </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -9504,6 +9913,9 @@
       <c r="Q67">
         <v>86</v>
       </c>
+      <c r="R67">
+        <v>89</v>
+      </c>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -9557,111 +9969,120 @@
       <c r="Q68">
         <v>74</v>
       </c>
+      <c r="R68">
+        <v>81</v>
+      </c>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B69" s="5">
-        <v>19.172005914243471</v>
+        <v>1.9762845849802373</v>
       </c>
       <c r="C69">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D69">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E69">
+        <v>4</v>
+      </c>
+      <c r="F69">
+        <v>6</v>
+      </c>
+      <c r="G69">
+        <v>8</v>
+      </c>
+      <c r="H69">
+        <v>10</v>
+      </c>
+      <c r="I69">
+        <v>10</v>
+      </c>
+      <c r="J69">
+        <v>11</v>
+      </c>
+      <c r="K69">
+        <v>14</v>
+      </c>
+      <c r="L69">
+        <v>18</v>
+      </c>
+      <c r="M69">
         <v>24</v>
       </c>
-      <c r="F69">
-        <v>26</v>
-      </c>
-      <c r="G69">
-        <v>28</v>
-      </c>
-      <c r="H69">
-        <v>29</v>
-      </c>
-      <c r="I69">
-        <v>31</v>
-      </c>
-      <c r="J69">
-        <v>33</v>
-      </c>
-      <c r="K69">
-        <v>34</v>
-      </c>
-      <c r="L69">
-        <v>36</v>
-      </c>
-      <c r="M69">
+      <c r="N69">
+        <v>30</v>
+      </c>
+      <c r="O69">
+        <v>35</v>
+      </c>
+      <c r="P69">
         <v>37</v>
       </c>
-      <c r="N69">
-        <v>39</v>
-      </c>
-      <c r="O69">
-        <v>41</v>
-      </c>
-      <c r="P69">
-        <v>43</v>
-      </c>
       <c r="Q69">
-        <v>46</v>
+        <v>40</v>
+      </c>
+      <c r="R69">
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B70" s="5">
-        <v>1.9762845849802373</v>
+        <v>19.172005914243471</v>
       </c>
       <c r="C70">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E70">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F70">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G70">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="H70">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="I70">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="J70">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="K70">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="L70">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="M70">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="N70">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="O70">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="P70">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="Q70">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="R70">
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.2">
@@ -9716,6 +10137,9 @@
       <c r="Q71">
         <v>32</v>
       </c>
+      <c r="R71">
+        <v>33</v>
+      </c>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
@@ -9768,6 +10192,9 @@
       </c>
       <c r="Q72">
         <v>29</v>
+      </c>
+      <c r="R72">
+        <v>33</v>
       </c>
       <c r="AD72" s="5"/>
       <c r="AR72" s="5"/>
@@ -9824,6 +10251,9 @@
       <c r="Q73">
         <v>23</v>
       </c>
+      <c r="R73">
+        <v>25</v>
+      </c>
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
@@ -9877,6 +10307,9 @@
       <c r="Q74">
         <v>19</v>
       </c>
+      <c r="R74">
+        <v>22</v>
+      </c>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
@@ -9930,6 +10363,9 @@
       <c r="Q75">
         <v>13</v>
       </c>
+      <c r="R75">
+        <v>14</v>
+      </c>
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -9983,6 +10419,9 @@
       <c r="Q76">
         <v>7</v>
       </c>
+      <c r="R76">
+        <v>9</v>
+      </c>
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
@@ -10036,46 +10475,49 @@
       <c r="Q77">
         <v>4</v>
       </c>
+      <c r="R77">
+        <v>4</v>
+      </c>
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B78" s="5">
         <v>0</v>
       </c>
-      <c r="B78" s="5">
-        <v>2.3484848484848486</v>
-      </c>
       <c r="C78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N78">
         <v>2</v>
@@ -10088,47 +10530,50 @@
       </c>
       <c r="Q78">
         <v>2</v>
+      </c>
+      <c r="R78">
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B79" s="5">
-        <v>0</v>
+        <v>2.3484848484848486</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N79">
         <v>2</v>
@@ -10140,6 +10585,9 @@
         <v>2</v>
       </c>
       <c r="Q79">
+        <v>2</v>
+      </c>
+      <c r="R79">
         <v>2</v>
       </c>
     </row>
@@ -10195,10 +10643,13 @@
       <c r="Q80">
         <v>1</v>
       </c>
+      <c r="R80">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:Q80">
-    <sortCondition descending="1" ref="Q62:Q80"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:R80">
+    <sortCondition descending="1" ref="R62:R80"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B25:C25"/>
@@ -10223,25 +10674,25 @@
     <hyperlink ref="A43" r:id="rId17" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{2749059A-A8E1-B840-90D7-560A71410172}"/>
     <hyperlink ref="A29" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
     <hyperlink ref="A27" r:id="rId19" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{57A3EA1C-224C-3F47-BBF4-F96842A83158}"/>
-    <hyperlink ref="A36" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
+    <hyperlink ref="A34" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
     <hyperlink ref="A33" r:id="rId21" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{AB6442DB-502D-BF47-BD97-FD78208EA473}"/>
-    <hyperlink ref="A38" r:id="rId22" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{E8933148-C5A5-C049-998E-8A19BCC472EE}"/>
+    <hyperlink ref="A39" r:id="rId22" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{E8933148-C5A5-C049-998E-8A19BCC472EE}"/>
     <hyperlink ref="A31" r:id="rId23" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{148898F7-DFEC-AD49-AE18-589CAE84737B}"/>
     <hyperlink ref="A42" r:id="rId24" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{C028FE55-7852-3F41-9817-549C985F7260}"/>
     <hyperlink ref="A28" r:id="rId25" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{B5BDCE1C-B9BF-5D4E-AF41-63D149E1115B}"/>
-    <hyperlink ref="A39" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
+    <hyperlink ref="A38" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
     <hyperlink ref="A35" r:id="rId27" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{D6541E56-79D1-DD4C-89C0-B9FE943CF17D}"/>
     <hyperlink ref="A32" r:id="rId28" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{DB82E052-EA56-4542-B5D9-CDCA3F75C63F}"/>
     <hyperlink ref="A30" r:id="rId29" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{B76E0484-5117-5040-B058-D17B21DC5420}"/>
-    <hyperlink ref="A34" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
+    <hyperlink ref="A36" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
     <hyperlink ref="A40" r:id="rId31" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{219CBCE6-9D2C-5146-B0CA-29FE2A0FA513}"/>
     <hyperlink ref="A41" r:id="rId32" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{A66187B1-4AD9-444B-BCFA-FF8464EDFF33}"/>
-    <hyperlink ref="A78" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
+    <hyperlink ref="A79" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
     <hyperlink ref="A63" r:id="rId34" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{A20FB0CD-F9DA-914E-B2F5-F280E65964E3}"/>
     <hyperlink ref="A62" r:id="rId35" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{EE62FA68-128F-064D-A4F8-F9BE8B79FC59}"/>
     <hyperlink ref="A72" r:id="rId36" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{D2FB73FA-EC57-274E-BF29-C09B1AC3DDE2}"/>
     <hyperlink ref="A74" r:id="rId37" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{523B8969-55CC-FF4F-9FA9-106BC6D662B5}"/>
-    <hyperlink ref="A69" r:id="rId38" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{517487C3-ADE3-274F-9F6E-78AC36F61827}"/>
+    <hyperlink ref="A70" r:id="rId38" display="https://www.worldometers.info/coronavirus/country/iran/" xr:uid="{517487C3-ADE3-274F-9F6E-78AC36F61827}"/>
     <hyperlink ref="A65" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
     <hyperlink ref="A77" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
     <hyperlink ref="A67" r:id="rId41" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{92D1F4A4-B981-3C45-A55A-E63BE05C7D4F}"/>
@@ -10250,7 +10701,7 @@
     <hyperlink ref="A73" r:id="rId44" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{76C0B263-3E56-DD44-BF90-D7A725F4C11B}"/>
     <hyperlink ref="A64" r:id="rId45" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{F788A2F0-F76C-0A46-84F6-32311CDCE6EB}"/>
     <hyperlink ref="A75" r:id="rId46" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{1FA4FB2B-21FB-A240-B716-855DE4CC3FCA}"/>
-    <hyperlink ref="A70" r:id="rId47" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{52773F30-B0DE-FE41-B798-80BFDD6B52F9}"/>
+    <hyperlink ref="A69" r:id="rId47" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{52773F30-B0DE-FE41-B798-80BFDD6B52F9}"/>
     <hyperlink ref="A76" r:id="rId48" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{03FEC42E-DDC8-9B40-8CF7-F008D15BED91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update 12 April II
</commit_message>
<xml_diff>
--- a/COVID19 calculos.xlsx
+++ b/COVID19 calculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rramirez/projects/COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923E5842-74BD-494B-AEDC-E4592A06C169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BAEB18-CDC4-634B-8DF7-43D638F69CD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="49">
   <si>
     <t>China</t>
   </si>
@@ -178,6 +178,9 @@
   <si>
     <t>11 April</t>
   </si>
+  <si>
+    <t>12 April</t>
+  </si>
 </sst>
 </file>
 
@@ -223,18 +226,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -257,7 +254,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -269,11 +266,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -410,10 +406,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -431,10 +427,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -476,10 +472,10 @@
                   <c:v>800.81680280046669</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>246.92982456140351</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>885.87962962962968</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>246.92982456140351</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>215.83818480370206</c:v>
@@ -497,10 +493,10 @@
                   <c:v>211.35040745052387</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>75.526791089705</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>403.12965722801783</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>75.526791089705</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>251</c:v>
@@ -571,10 +567,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -592,10 +588,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -637,10 +633,10 @@
                   <c:v>872.11201866977831</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>977.81084656084658</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>239</c:v>
@@ -658,10 +654,10 @@
                   <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>421.5722801788375</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>262</c:v>
@@ -732,10 +728,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -753,10 +749,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -798,10 +794,10 @@
                   <c:v>997</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1057</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>328</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>296</c:v>
@@ -819,10 +815,10 @@
                   <c:v>276</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>474</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>282</c:v>
@@ -893,10 +889,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -914,10 +910,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -958,11 +954,11 @@
                 <c:pt idx="1">
                   <c:v>1153</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1144</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>374</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>333</c:v>
@@ -980,10 +976,10 @@
                   <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>518</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>284</c:v>
@@ -1054,10 +1050,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -1075,10 +1071,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -1119,11 +1115,11 @@
                 <c:pt idx="1">
                   <c:v>1272</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1230</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>433</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>377</c:v>
@@ -1141,10 +1137,10 @@
                   <c:v>373</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>571</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>308</c:v>
@@ -1215,10 +1211,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -1236,10 +1232,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -1280,11 +1276,11 @@
                 <c:pt idx="1">
                   <c:v>1378</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1332</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>547</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>435</c:v>
@@ -1302,10 +1298,10 @@
                   <c:v>433</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>628</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>335</c:v>
@@ -1378,10 +1374,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -1399,10 +1395,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -1443,11 +1439,11 @@
                 <c:pt idx="1">
                   <c:v>1509</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1430</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>639</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>492</c:v>
@@ -1465,10 +1461,10 @@
                   <c:v>501</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>628</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>365</c:v>
@@ -1541,10 +1537,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -1562,10 +1558,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -1606,11 +1602,11 @@
                 <c:pt idx="1">
                   <c:v>1642</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1529</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>801</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>561</c:v>
@@ -1628,10 +1624,10 @@
                   <c:v>568</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>748</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>393</c:v>
@@ -1704,10 +1700,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -1725,10 +1721,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -1769,11 +1765,11 @@
                 <c:pt idx="1">
                   <c:v>1730</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>951</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1615</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>951</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>600</c:v>
@@ -1791,10 +1787,10 @@
                   <c:v>632</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>758</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>428</c:v>
@@ -1867,10 +1863,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -1888,10 +1884,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -1932,11 +1928,11 @@
                 <c:pt idx="1">
                   <c:v>1858</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1044</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1682</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1044</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>665</c:v>
@@ -1954,10 +1950,10 @@
                   <c:v>624</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>828</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>333</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>460</c:v>
@@ -2030,10 +2026,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -2051,10 +2047,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -2095,11 +2091,11 @@
                 <c:pt idx="1">
                   <c:v>1938</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1121</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1749</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1121</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>778</c:v>
@@ -2117,10 +2113,10 @@
                   <c:v>733</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>865</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>511</c:v>
@@ -2193,10 +2189,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -2214,10 +2210,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -2258,11 +2254,11 @@
                 <c:pt idx="1">
                   <c:v>2073</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1225</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1828</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1225</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>851</c:v>
@@ -2280,10 +2276,10 @@
                   <c:v>792</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>909</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>444</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>555</c:v>
@@ -2357,10 +2353,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -2378,10 +2374,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -2422,11 +2418,11 @@
                 <c:pt idx="1">
                   <c:v>2197</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1346</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1905</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1346</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>882</c:v>
@@ -2444,10 +2440,10 @@
                   <c:v>855</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>959</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>507</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>605</c:v>
@@ -2521,10 +2517,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -2542,10 +2538,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -2586,11 +2582,11 @@
                 <c:pt idx="1">
                   <c:v>2288</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1471</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>1981</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1471</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>960</c:v>
@@ -2608,10 +2604,10 @@
                   <c:v>915</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>574</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>671</c:v>
@@ -2685,10 +2681,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -2706,10 +2702,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -2750,11 +2746,11 @@
                 <c:pt idx="1">
                   <c:v>2393</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1617</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2061</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1617</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1343</c:v>
@@ -2772,10 +2768,10 @@
                   <c:v>968</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1034</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>631</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>728</c:v>
@@ -2849,10 +2845,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -2870,10 +2866,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -2914,11 +2910,11 @@
                 <c:pt idx="1">
                   <c:v>2483</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1826</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2132</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1826</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1386</c:v>
@@ -2936,10 +2932,10 @@
                   <c:v>1039</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1059</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>780</c:v>
@@ -3013,10 +3009,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -3034,10 +3030,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -3078,11 +3074,11 @@
                 <c:pt idx="1">
                   <c:v>2527</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1826</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2192</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1826</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1463</c:v>
@@ -3100,10 +3096,10 @@
                   <c:v>1094</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1093</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>777</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>836</c:v>
@@ -3177,10 +3173,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -3198,10 +3194,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -3242,11 +3238,11 @@
                 <c:pt idx="1">
                   <c:v>2597</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>1947</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2242</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1947</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1628</c:v>
@@ -3264,10 +3260,10 @@
                   <c:v>1140</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>831</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1134</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>831</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>906</c:v>
@@ -3340,10 +3336,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -3361,10 +3357,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -3405,11 +3401,11 @@
                 <c:pt idx="1">
                   <c:v>2716</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>2053</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2305</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2053</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1686</c:v>
@@ -3427,10 +3423,10 @@
                   <c:v>1196</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1126</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>914</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>965</c:v>
@@ -3503,10 +3499,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -3524,10 +3520,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -3568,11 +3564,11 @@
                 <c:pt idx="1">
                   <c:v>2806</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>2191</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2375</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2191</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1758</c:v>
@@ -3590,10 +3586,10 @@
                   <c:v>1267</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>979</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1159</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>979</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1006</c:v>
@@ -3666,10 +3662,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -3687,10 +3683,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -3731,11 +3727,11 @@
                 <c:pt idx="1">
                   <c:v>2865</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>2339</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2440</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2339</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1864</c:v>
@@ -3753,10 +3749,10 @@
                   <c:v>1344</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1193</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1110</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1039</c:v>
@@ -3829,10 +3825,10 @@
                   <c:v>Switzerland</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Italy</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Belgium</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>France</c:v>
@@ -3850,10 +3846,10 @@
                   <c:v>Netherlands</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Norway</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Denmark</c:v>
@@ -3894,11 +3890,11 @@
                 <c:pt idx="1">
                   <c:v>2930</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0">
+                <c:pt idx="2">
+                  <c:v>2458</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
                   <c:v>2518</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2458</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1935</c:v>
@@ -3916,10 +3912,10 @@
                   <c:v>1421</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>1189</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>1194</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1189</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1071</c:v>
@@ -3951,6 +3947,169 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-34C2-A44A-93EB-83FBC4FA48EB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="22"/>
+          <c:order val="22"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$X$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12 April</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$27:$A$45</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$X$27:$X$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3575</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2966</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2601</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0">
+                  <c:v>2585</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1713</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1581</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1544</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1489</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1268</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1216</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1036</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>883</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-34C2-A44A-93EB-83FBC4FA48EB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4308,10 +4467,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -4374,10 +4533,10 @@
                   <c:v>8.3893118375876998</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3.5069235400361229</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>7.9161816065192081</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5069235400361229</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9.3348891481913654</c:v>
@@ -4469,10 +4628,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -4535,10 +4694,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
                   <c:v>11</c:v>
@@ -4630,10 +4789,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -4696,10 +4855,10 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>14</c:v>
@@ -4791,10 +4950,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -4857,10 +5016,10 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>14</c:v>
@@ -4952,10 +5111,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -5018,10 +5177,10 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>18</c:v>
@@ -5113,10 +5272,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -5179,10 +5338,10 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>22</c:v>
@@ -5276,10 +5435,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -5342,10 +5501,10 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>27</c:v>
@@ -5439,10 +5598,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -5505,10 +5664,10 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>31</c:v>
@@ -5602,10 +5761,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -5668,10 +5827,10 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>35</c:v>
@@ -5765,10 +5924,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -5831,10 +5990,10 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>42</c:v>
@@ -5928,10 +6087,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -5994,10 +6153,10 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>51</c:v>
@@ -6091,10 +6250,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -6157,10 +6316,10 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>57</c:v>
@@ -6255,10 +6414,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -6321,10 +6480,10 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>63</c:v>
@@ -6419,10 +6578,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -6485,10 +6644,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>69</c:v>
@@ -6583,10 +6742,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -6649,10 +6808,10 @@
                   <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>78</c:v>
@@ -6747,10 +6906,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -6813,10 +6972,10 @@
                   <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>103</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>86</c:v>
@@ -6911,10 +7070,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -6977,10 +7136,10 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>109</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>89</c:v>
@@ -7075,10 +7234,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -7141,10 +7300,10 @@
                   <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>96</c:v>
@@ -7238,10 +7397,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -7304,10 +7463,10 @@
                   <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>104</c:v>
@@ -7401,10 +7560,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -7467,10 +7626,10 @@
                   <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>139</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>111</c:v>
@@ -7564,10 +7723,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -7630,10 +7789,10 @@
                   <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>146</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>117</c:v>
@@ -7727,10 +7886,10 @@
                   <c:v>France</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Netherlands</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>UK</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Switzerland</c:v>
@@ -7793,10 +7952,10 @@
                   <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>154</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>121</c:v>
@@ -7843,6 +8002,169 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2B7C-9C4E-85DA-26C64BF5B6F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="22"/>
+          <c:order val="22"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$X$61</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12 April</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Calculos COVID19'!$A$62:$A$80</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Iran</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>S. Korea</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Colombia</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Calculos COVID19'!$X$62:$X$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2B7C-9C4E-85DA-26C64BF5B6F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9511,8 +9833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3BD7B-3B40-A94B-99F4-AAD0A2BEB996}">
   <dimension ref="A1:AR80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Z52" sqref="Z52"/>
+    <sheetView tabSelected="1" topLeftCell="O48" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Y58" sqref="Y58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9550,80 +9872,78 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>81953</v>
+        <v>82160</v>
       </c>
       <c r="C2" s="2">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2">
-        <v>3339</v>
+        <v>3341</v>
       </c>
       <c r="E2" s="3">
         <v>1386</v>
       </c>
       <c r="F2" s="5">
         <f>B2/E2</f>
-        <v>59.129148629148631</v>
+        <v>59.278499278499275</v>
       </c>
       <c r="G2" s="5">
         <f>D2/E2</f>
-        <v>2.4090909090909092</v>
+        <v>2.4105339105339105</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>152271</v>
+        <v>156363</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
-        <v>19468</v>
+        <v>19899</v>
       </c>
       <c r="E3" s="4">
         <v>60.48</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F20" si="0">B3/E3</f>
-        <v>2517.7083333333335</v>
+        <v>2585.3670634920636</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" ref="G3:G19" si="1">D3/E3</f>
-        <v>321.89153439153444</v>
+        <v>329.01785714285717</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>163027</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2992</v>
-      </c>
+        <v>166831</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2">
-        <v>16606</v>
+        <v>17209</v>
       </c>
       <c r="E4" s="4">
         <v>46.66</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="0"/>
-        <v>3493.9348478354054</v>
+        <v>3575.4607801114448</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="1"/>
-        <v>355.89369909987141</v>
+        <v>368.81697385340766</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -9632,132 +9952,130 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>533115</v>
+        <v>560433</v>
       </c>
       <c r="C5" s="2">
-        <v>236</v>
+        <v>133</v>
       </c>
       <c r="D5" s="2">
-        <v>20580</v>
+        <v>22115</v>
       </c>
       <c r="E5" s="4">
         <v>327.2</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>1629.3245721271394</v>
+        <v>1712.8147921760392</v>
       </c>
       <c r="G5" s="5">
         <f>D5/E5</f>
-        <v>62.897310513447437</v>
+        <v>67.58863080684597</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>125452</v>
+        <v>127854</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
-        <v>2871</v>
+        <v>3022</v>
       </c>
       <c r="E6" s="4">
         <v>82.79</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>1515.3037806498369</v>
+        <v>1544.3169464911221</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>34.678101219954101</v>
+        <v>36.501992994322983</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>70029</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1657</v>
-      </c>
+        <v>71686</v>
+      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2">
-        <v>4357</v>
+        <v>4474</v>
       </c>
       <c r="E7" s="4">
         <v>81.16</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>862.85115820601288</v>
+        <v>883.26761951700348</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="1"/>
-        <v>53.684080827994087</v>
+        <v>55.125677673730905</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>129654</v>
+        <v>132591</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
-        <v>13832</v>
+        <v>14393</v>
       </c>
       <c r="E8" s="4">
         <v>66.989999999999995</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>1935.4231974921631</v>
+        <v>1979.2655620241828</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="1"/>
-        <v>206.47857889237201</v>
+        <v>214.85296312882522</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>10480</v>
+        <v>10537</v>
       </c>
       <c r="C9" s="2">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E9" s="4">
         <v>51.47</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>203.61375558577814</v>
+        <v>204.72119681367786</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="1"/>
-        <v>4.0994754225762584</v>
+        <v>4.2160481834078105</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -9765,287 +10083,273 @@
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>25107</v>
-      </c>
-      <c r="C10" s="2">
-        <v>193</v>
-      </c>
+        <v>25415</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2">
-        <v>1036</v>
+        <v>1106</v>
       </c>
       <c r="E10" s="4">
         <v>8.57</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>2929.6382730455075</v>
+        <v>2965.5775962660441</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="1"/>
-        <v>120.88681446907817</v>
+        <v>129.05484247374562</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>78991</v>
+        <v>84279</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
-        <v>9875</v>
+        <v>10612</v>
       </c>
       <c r="E11" s="4">
         <v>66.44</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>1188.9072847682119</v>
+        <v>1268.4978928356413</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="1"/>
-        <v>148.63034316676701</v>
+        <v>159.72305839855508</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>24413</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1174</v>
-      </c>
+        <v>25587</v>
+      </c>
+      <c r="C12" s="2"/>
       <c r="D12" s="2">
-        <v>2643</v>
+        <v>2737</v>
       </c>
       <c r="E12" s="4">
         <v>17.18</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>1421.0128055878929</v>
+        <v>1489.348079161816</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="1"/>
-        <v>153.84167636786961</v>
+        <v>159.31315483119909</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>13806</v>
-      </c>
-      <c r="C13" s="2">
-        <v>139</v>
-      </c>
+        <v>13945</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="E13" s="4">
         <v>8.82</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>1565.3061224489795</v>
+        <v>1581.0657596371882</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="1"/>
-        <v>38.208616780045354</v>
+        <v>39.682539682539684</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>28018</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1629</v>
-      </c>
+        <v>29647</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2">
-        <v>3346</v>
+        <v>3600</v>
       </c>
       <c r="E14" s="4">
         <v>11.4</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>2457.719298245614</v>
+        <v>2600.614035087719</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="1"/>
-        <v>293.50877192982455</v>
+        <v>315.78947368421052</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>6409</v>
-      </c>
-      <c r="C15" s="2">
-        <v>50</v>
-      </c>
+        <v>6525</v>
+      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="E15" s="4">
         <v>5.3680000000000003</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="0"/>
-        <v>1193.9269746646796</v>
+        <v>1215.5365126676602</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="1"/>
-        <v>22.168405365126674</v>
+        <v>23.845007451564829</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>10151</v>
-      </c>
-      <c r="C16" s="2">
-        <v>332</v>
-      </c>
+        <v>10483</v>
+      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2">
-        <v>887</v>
+        <v>899</v>
       </c>
       <c r="E16" s="4">
         <v>10.119999999999999</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>1003.0632411067195</v>
+        <v>1035.8695652173915</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="1"/>
-        <v>87.64822134387353</v>
+        <v>88.833992094861671</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2">
-        <v>23318</v>
+        <v>24383</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
-        <v>653</v>
+        <v>717</v>
       </c>
       <c r="E17" s="4">
         <v>37.590000000000003</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>620.32455440276669</v>
+        <v>648.65655759510503</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="1"/>
-        <v>17.371641393987762</v>
+        <v>19.074221867517956</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>2709</v>
+        <v>2776</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E18" s="4">
         <v>49.07</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="0"/>
-        <v>55.206847360912981</v>
+        <v>56.572243733442022</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="1"/>
-        <v>2.037905033625433</v>
+        <v>2.2213164866517219</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="2">
-        <v>5996</v>
-      </c>
-      <c r="C19" s="2">
-        <v>178</v>
-      </c>
+        <v>6174</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2">
-        <v>260</v>
+        <v>273</v>
       </c>
       <c r="E19" s="4">
         <v>5.6</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="0"/>
-        <v>1070.7142857142858</v>
+        <v>1102.5</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" si="1"/>
-        <v>46.428571428571431</v>
+        <v>48.75</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>20962</v>
+        <v>22318</v>
       </c>
       <c r="C20" s="2">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="D20" s="2">
-        <v>1140</v>
+        <v>1230</v>
       </c>
       <c r="E20" s="4">
         <v>209.3</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="0"/>
-        <v>100.15289058767318</v>
+        <v>106.63162924032488</v>
       </c>
       <c r="G20" s="5">
         <f>D20/E20</f>
-        <v>5.4467271858576201</v>
+        <v>5.8767319636884849</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -10054,7 +10358,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -10063,7 +10367,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -10072,14 +10376,14 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -10149,8 +10453,11 @@
       <c r="W26" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="X26" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -10220,8 +10527,11 @@
       <c r="W27">
         <v>3494</v>
       </c>
+      <c r="X27">
+        <v>3575</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -10291,150 +10601,159 @@
       <c r="W28">
         <v>2930</v>
       </c>
+      <c r="X28">
+        <v>2966</v>
+      </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="5">
+        <v>246.92982456140351</v>
+      </c>
+      <c r="C29" s="5">
+        <v>298</v>
+      </c>
+      <c r="D29">
+        <v>328</v>
+      </c>
+      <c r="E29">
+        <v>374</v>
+      </c>
+      <c r="F29">
+        <v>433</v>
+      </c>
+      <c r="G29">
+        <v>547</v>
+      </c>
+      <c r="H29">
+        <v>639</v>
+      </c>
+      <c r="I29">
+        <v>801</v>
+      </c>
+      <c r="J29">
+        <v>951</v>
+      </c>
+      <c r="K29">
+        <v>1044</v>
+      </c>
+      <c r="L29">
+        <v>1121</v>
+      </c>
+      <c r="M29">
+        <v>1225</v>
+      </c>
+      <c r="N29">
+        <v>1346</v>
+      </c>
+      <c r="O29">
+        <v>1471</v>
+      </c>
+      <c r="P29">
+        <v>1617</v>
+      </c>
+      <c r="Q29">
+        <v>1826</v>
+      </c>
+      <c r="R29">
+        <v>1826</v>
+      </c>
+      <c r="S29">
+        <v>1947</v>
+      </c>
+      <c r="T29">
+        <v>2053</v>
+      </c>
+      <c r="U29">
+        <v>2191</v>
+      </c>
+      <c r="V29">
+        <v>2339</v>
+      </c>
+      <c r="W29">
+        <v>2458</v>
+      </c>
+      <c r="X29">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B30" s="5">
         <v>885.87962962962968</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C30" s="5">
         <v>977.81084656084658</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>1057</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E30" s="5">
         <v>1144</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F30" s="5">
         <v>1230</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G30" s="5">
         <v>1332</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H30" s="5">
         <v>1430</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I30" s="5">
         <v>1529</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J30" s="5">
         <v>1615</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K30" s="5">
         <v>1682</v>
       </c>
-      <c r="L29" s="5">
+      <c r="L30" s="5">
         <v>1749</v>
       </c>
-      <c r="M29" s="5">
+      <c r="M30" s="5">
         <v>1828</v>
       </c>
-      <c r="N29" s="5">
+      <c r="N30" s="5">
         <v>1905</v>
       </c>
-      <c r="O29" s="5">
+      <c r="O30" s="5">
         <v>1981</v>
       </c>
-      <c r="P29" s="5">
+      <c r="P30" s="5">
         <v>2061</v>
       </c>
-      <c r="Q29" s="5">
+      <c r="Q30" s="5">
         <v>2132</v>
       </c>
-      <c r="R29" s="5">
+      <c r="R30" s="5">
         <v>2192</v>
       </c>
-      <c r="S29" s="5">
+      <c r="S30" s="5">
         <v>2242</v>
       </c>
-      <c r="T29" s="5">
+      <c r="T30" s="5">
         <v>2305</v>
       </c>
-      <c r="U29" s="5">
+      <c r="U30" s="5">
         <v>2375</v>
       </c>
-      <c r="V29" s="5">
+      <c r="V30" s="5">
         <v>2440</v>
       </c>
-      <c r="W29" s="5">
+      <c r="W30" s="5">
         <v>2518</v>
       </c>
+      <c r="X30" s="5">
+        <v>2585</v>
+      </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="5">
-        <v>246.92982456140351</v>
-      </c>
-      <c r="C30" s="5">
-        <v>298</v>
-      </c>
-      <c r="D30">
-        <v>328</v>
-      </c>
-      <c r="E30">
-        <v>374</v>
-      </c>
-      <c r="F30">
-        <v>433</v>
-      </c>
-      <c r="G30">
-        <v>547</v>
-      </c>
-      <c r="H30">
-        <v>639</v>
-      </c>
-      <c r="I30">
-        <v>801</v>
-      </c>
-      <c r="J30">
-        <v>951</v>
-      </c>
-      <c r="K30">
-        <v>1044</v>
-      </c>
-      <c r="L30">
-        <v>1121</v>
-      </c>
-      <c r="M30">
-        <v>1225</v>
-      </c>
-      <c r="N30">
-        <v>1346</v>
-      </c>
-      <c r="O30">
-        <v>1471</v>
-      </c>
-      <c r="P30">
-        <v>1617</v>
-      </c>
-      <c r="Q30">
-        <v>1826</v>
-      </c>
-      <c r="R30">
-        <v>1826</v>
-      </c>
-      <c r="S30">
-        <v>1947</v>
-      </c>
-      <c r="T30">
-        <v>2053</v>
-      </c>
-      <c r="U30">
-        <v>2191</v>
-      </c>
-      <c r="V30">
-        <v>2339</v>
-      </c>
-      <c r="W30">
-        <v>2458</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -10504,8 +10823,11 @@
       <c r="W31">
         <v>1935</v>
       </c>
+      <c r="X31">
+        <v>1979</v>
+      </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -10575,8 +10897,11 @@
       <c r="W32">
         <v>1629</v>
       </c>
+      <c r="X32">
+        <v>1713</v>
+      </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -10646,8 +10971,11 @@
       <c r="W33">
         <v>1565</v>
       </c>
+      <c r="X33">
+        <v>1581</v>
+      </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -10717,8 +11045,11 @@
       <c r="W34">
         <v>1515</v>
       </c>
+      <c r="X34">
+        <v>1544</v>
+      </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -10788,150 +11119,159 @@
       <c r="W35">
         <v>1421</v>
       </c>
+      <c r="X35">
+        <v>1489</v>
+      </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5">
+        <v>75.526791089705</v>
+      </c>
+      <c r="C36" s="5">
+        <v>86</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+      <c r="E36">
+        <v>122</v>
+      </c>
+      <c r="F36">
+        <v>198</v>
+      </c>
+      <c r="G36">
+        <v>175</v>
+      </c>
+      <c r="H36">
+        <v>219</v>
+      </c>
+      <c r="I36">
+        <v>257</v>
+      </c>
+      <c r="J36">
+        <v>294</v>
+      </c>
+      <c r="K36">
+        <v>333</v>
+      </c>
+      <c r="L36">
+        <v>379</v>
+      </c>
+      <c r="M36">
+        <v>444</v>
+      </c>
+      <c r="N36">
+        <v>507</v>
+      </c>
+      <c r="O36">
+        <v>574</v>
+      </c>
+      <c r="P36">
+        <v>631</v>
+      </c>
+      <c r="Q36">
+        <v>720</v>
+      </c>
+      <c r="R36">
+        <v>777</v>
+      </c>
+      <c r="S36">
+        <v>831</v>
+      </c>
+      <c r="T36">
+        <v>914</v>
+      </c>
+      <c r="U36">
+        <v>979</v>
+      </c>
+      <c r="V36">
+        <v>1110</v>
+      </c>
+      <c r="W36">
+        <v>1189</v>
+      </c>
+      <c r="X36">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B37" s="5">
         <v>403.12965722801783</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C37" s="5">
         <v>421.5722801788375</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>474</v>
       </c>
-      <c r="E36">
+      <c r="E37">
         <v>518</v>
       </c>
-      <c r="F36">
+      <c r="F37">
         <v>571</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <v>628</v>
       </c>
-      <c r="H36">
+      <c r="H37">
         <v>628</v>
       </c>
-      <c r="I36">
+      <c r="I37">
         <v>748</v>
       </c>
-      <c r="J36">
+      <c r="J37">
         <v>758</v>
       </c>
-      <c r="K36">
+      <c r="K37">
         <v>828</v>
       </c>
-      <c r="L36">
+      <c r="L37">
         <v>865</v>
       </c>
-      <c r="M36">
+      <c r="M37">
         <v>909</v>
       </c>
-      <c r="N36">
+      <c r="N37">
         <v>959</v>
       </c>
-      <c r="O36">
+      <c r="O37">
         <v>1000</v>
       </c>
-      <c r="P36">
+      <c r="P37">
         <v>1034</v>
       </c>
-      <c r="Q36">
+      <c r="Q37">
         <v>1059</v>
       </c>
-      <c r="R36">
+      <c r="R37">
         <v>1093</v>
       </c>
-      <c r="S36">
+      <c r="S37">
         <v>1134</v>
       </c>
-      <c r="T36">
+      <c r="T37">
         <v>1126</v>
       </c>
-      <c r="U36">
+      <c r="U37">
         <v>1159</v>
       </c>
-      <c r="V36">
+      <c r="V37">
         <v>1193</v>
       </c>
-      <c r="W36">
+      <c r="W37">
         <v>1194</v>
       </c>
+      <c r="X37">
+        <v>1216</v>
+      </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="5">
-        <v>75.526791089705</v>
-      </c>
-      <c r="C37" s="5">
-        <v>86</v>
-      </c>
-      <c r="D37">
-        <v>100</v>
-      </c>
-      <c r="E37">
-        <v>122</v>
-      </c>
-      <c r="F37">
-        <v>198</v>
-      </c>
-      <c r="G37">
-        <v>175</v>
-      </c>
-      <c r="H37">
-        <v>219</v>
-      </c>
-      <c r="I37">
-        <v>257</v>
-      </c>
-      <c r="J37">
-        <v>294</v>
-      </c>
-      <c r="K37">
-        <v>333</v>
-      </c>
-      <c r="L37">
-        <v>379</v>
-      </c>
-      <c r="M37">
-        <v>444</v>
-      </c>
-      <c r="N37">
-        <v>507</v>
-      </c>
-      <c r="O37">
-        <v>574</v>
-      </c>
-      <c r="P37">
-        <v>631</v>
-      </c>
-      <c r="Q37">
-        <v>720</v>
-      </c>
-      <c r="R37">
-        <v>777</v>
-      </c>
-      <c r="S37">
-        <v>831</v>
-      </c>
-      <c r="T37">
-        <v>914</v>
-      </c>
-      <c r="U37">
-        <v>979</v>
-      </c>
-      <c r="V37">
-        <v>1110</v>
-      </c>
-      <c r="W37">
-        <v>1189</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
@@ -11001,8 +11341,11 @@
       <c r="W38">
         <v>1071</v>
       </c>
+      <c r="X38">
+        <v>1103</v>
+      </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
@@ -11072,8 +11415,11 @@
       <c r="W39">
         <v>1003</v>
       </c>
+      <c r="X39">
+        <v>1036</v>
+      </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
@@ -11143,8 +11489,11 @@
       <c r="W40">
         <v>863</v>
       </c>
+      <c r="X40">
+        <v>883</v>
+      </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -11214,8 +11563,11 @@
       <c r="W41">
         <v>620</v>
       </c>
+      <c r="X41">
+        <v>649</v>
+      </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
@@ -11285,8 +11637,11 @@
       <c r="W42">
         <v>204</v>
       </c>
+      <c r="X42">
+        <v>205</v>
+      </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>29</v>
       </c>
@@ -11356,8 +11711,11 @@
       <c r="W43">
         <v>100</v>
       </c>
+      <c r="X43">
+        <v>107</v>
+      </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -11427,8 +11785,11 @@
       <c r="W44" s="5">
         <v>59</v>
       </c>
+      <c r="X44" s="5">
+        <v>59</v>
+      </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>22</v>
       </c>
@@ -11498,8 +11859,11 @@
       <c r="W45">
         <v>55</v>
       </c>
+      <c r="X45">
+        <v>57</v>
+      </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -11569,8 +11933,11 @@
       <c r="W61" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="X61" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>2</v>
       </c>
@@ -11640,8 +12007,11 @@
       <c r="W62">
         <v>356</v>
       </c>
+      <c r="X62">
+        <v>369</v>
+      </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
@@ -11711,8 +12081,11 @@
       <c r="W63">
         <v>322</v>
       </c>
+      <c r="X63">
+        <v>329</v>
+      </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>12</v>
       </c>
@@ -11781,6 +12154,9 @@
       </c>
       <c r="W64">
         <v>294</v>
+      </c>
+      <c r="X64">
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.2">
@@ -11853,147 +12229,156 @@
       <c r="W65">
         <v>206</v>
       </c>
+      <c r="X65">
+        <v>215</v>
+      </c>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B66" s="5">
-        <v>7.9161816065192081</v>
+        <v>3.5069235400361229</v>
       </c>
       <c r="C66">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D66">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E66">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F66">
+        <v>7</v>
+      </c>
+      <c r="G66">
+        <v>9</v>
+      </c>
+      <c r="H66">
+        <v>11</v>
+      </c>
+      <c r="I66">
+        <v>15</v>
+      </c>
+      <c r="J66">
+        <v>18</v>
+      </c>
+      <c r="K66">
         <v>21</v>
       </c>
-      <c r="G66">
-        <v>25</v>
-      </c>
-      <c r="H66">
-        <v>32</v>
-      </c>
-      <c r="I66">
-        <v>37</v>
-      </c>
-      <c r="J66">
-        <v>45</v>
-      </c>
-      <c r="K66">
-        <v>50</v>
-      </c>
       <c r="L66">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="M66">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="N66">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="O66">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="P66">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="Q66">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="R66">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="S66">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="T66">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="U66">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="V66">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="W66">
-        <v>154</v>
+        <v>149</v>
+      </c>
+      <c r="X66">
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B67" s="5">
-        <v>3.5069235400361229</v>
+        <v>7.9161816065192081</v>
       </c>
       <c r="C67">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E67">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F67">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G67">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="H67">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="I67">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="J67">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="K67">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="L67">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="M67">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="N67">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="O67">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="P67">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="Q67">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="R67">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="S67">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="T67">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="U67">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="V67">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="W67">
-        <v>149</v>
+        <v>154</v>
+      </c>
+      <c r="X67">
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.2">
@@ -12066,6 +12451,9 @@
       <c r="W68">
         <v>121</v>
       </c>
+      <c r="X68">
+        <v>129</v>
+      </c>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -12137,6 +12525,9 @@
       <c r="W69">
         <v>88</v>
       </c>
+      <c r="X69">
+        <v>89</v>
+      </c>
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
@@ -12208,6 +12599,9 @@
       <c r="W70">
         <v>63</v>
       </c>
+      <c r="X70">
+        <v>68</v>
+      </c>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
@@ -12279,6 +12673,9 @@
       <c r="W71">
         <v>54</v>
       </c>
+      <c r="X71">
+        <v>55</v>
+      </c>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
@@ -12349,6 +12746,9 @@
       </c>
       <c r="W72">
         <v>46</v>
+      </c>
+      <c r="X72">
+        <v>49</v>
       </c>
       <c r="AD72" s="5"/>
       <c r="AR72" s="5"/>
@@ -12423,6 +12823,9 @@
       <c r="W73">
         <v>38</v>
       </c>
+      <c r="X73">
+        <v>40</v>
+      </c>
     </row>
     <row r="74" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
@@ -12494,6 +12897,9 @@
       <c r="W74">
         <v>35</v>
       </c>
+      <c r="X74">
+        <v>37</v>
+      </c>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
@@ -12565,6 +12971,9 @@
       <c r="W75">
         <v>22</v>
       </c>
+      <c r="X75">
+        <v>24</v>
+      </c>
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -12636,6 +13045,9 @@
       <c r="W76">
         <v>17</v>
       </c>
+      <c r="X76">
+        <v>19</v>
+      </c>
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
@@ -12707,6 +13119,9 @@
       <c r="W77">
         <v>5</v>
       </c>
+      <c r="X77">
+        <v>6</v>
+      </c>
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
@@ -12778,6 +13193,9 @@
       <c r="W78">
         <v>4</v>
       </c>
+      <c r="X78">
+        <v>4</v>
+      </c>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
@@ -12849,6 +13267,9 @@
       <c r="W79">
         <v>2</v>
       </c>
+      <c r="X79">
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -12920,10 +13341,13 @@
       <c r="W80">
         <v>2</v>
       </c>
+      <c r="X80">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:W80">
-    <sortCondition descending="1" ref="W62:W80"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A62:X80">
+    <sortCondition descending="1" ref="X62:X80"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="B25:C25"/>
@@ -12946,7 +13370,7 @@
     <hyperlink ref="A16" r:id="rId15" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{6A5FA689-4530-FC48-8476-8EB82E5F1FB4}"/>
     <hyperlink ref="A17" r:id="rId16" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{768069AF-3C8F-EA44-BDE0-CFAD42D2AE89}"/>
     <hyperlink ref="A44" r:id="rId17" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{2749059A-A8E1-B840-90D7-560A71410172}"/>
-    <hyperlink ref="A29" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
+    <hyperlink ref="A30" r:id="rId18" display="https://www.worldometers.info/coronavirus/country/italy/" xr:uid="{C8A2C7E3-BCB6-5C46-B9C3-444096AF307B}"/>
     <hyperlink ref="A27" r:id="rId19" display="https://www.worldometers.info/coronavirus/country/spain/" xr:uid="{57A3EA1C-224C-3F47-BBF4-F96842A83158}"/>
     <hyperlink ref="A32" r:id="rId20" display="https://www.worldometers.info/coronavirus/country/us/" xr:uid="{DCFC442A-AD43-4641-B367-D34C694F68A8}"/>
     <hyperlink ref="A34" r:id="rId21" display="https://www.worldometers.info/coronavirus/country/germany/" xr:uid="{AB6442DB-502D-BF47-BD97-FD78208EA473}"/>
@@ -12954,11 +13378,11 @@
     <hyperlink ref="A31" r:id="rId23" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{148898F7-DFEC-AD49-AE18-589CAE84737B}"/>
     <hyperlink ref="A42" r:id="rId24" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{C028FE55-7852-3F41-9817-549C985F7260}"/>
     <hyperlink ref="A28" r:id="rId25" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{B5BDCE1C-B9BF-5D4E-AF41-63D149E1115B}"/>
-    <hyperlink ref="A37" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
+    <hyperlink ref="A36" r:id="rId26" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{74AFC393-BAA7-A24A-9C40-9468B146A781}"/>
     <hyperlink ref="A35" r:id="rId27" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{D6541E56-79D1-DD4C-89C0-B9FE943CF17D}"/>
     <hyperlink ref="A33" r:id="rId28" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{DB82E052-EA56-4542-B5D9-CDCA3F75C63F}"/>
-    <hyperlink ref="A30" r:id="rId29" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{B76E0484-5117-5040-B058-D17B21DC5420}"/>
-    <hyperlink ref="A36" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
+    <hyperlink ref="A29" r:id="rId29" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{B76E0484-5117-5040-B058-D17B21DC5420}"/>
+    <hyperlink ref="A37" r:id="rId30" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{45694200-AD74-0447-921B-98052D6217F2}"/>
     <hyperlink ref="A39" r:id="rId31" display="https://www.worldometers.info/coronavirus/country/sweden/" xr:uid="{219CBCE6-9D2C-5146-B0CA-29FE2A0FA513}"/>
     <hyperlink ref="A41" r:id="rId32" display="https://www.worldometers.info/coronavirus/country/canada/" xr:uid="{A66187B1-4AD9-444B-BCFA-FF8464EDFF33}"/>
     <hyperlink ref="A79" r:id="rId33" display="https://www.worldometers.info/coronavirus/country/china/" xr:uid="{1DC4F575-6382-4147-ADE9-62EB84FB4A0A}"/>
@@ -12970,8 +13394,8 @@
     <hyperlink ref="A65" r:id="rId39" display="https://www.worldometers.info/coronavirus/country/france/" xr:uid="{DF895D66-8035-D84B-8A55-69D49041CA73}"/>
     <hyperlink ref="A78" r:id="rId40" display="https://www.worldometers.info/coronavirus/country/south-korea/" xr:uid="{95A2796E-E8D5-9244-B105-B3F8CF8E3BB3}"/>
     <hyperlink ref="A68" r:id="rId41" display="https://www.worldometers.info/coronavirus/country/switzerland/" xr:uid="{92D1F4A4-B981-3C45-A55A-E63BE05C7D4F}"/>
-    <hyperlink ref="A67" r:id="rId42" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{9E857743-3BA1-D547-A532-A53EF891F862}"/>
-    <hyperlink ref="A66" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
+    <hyperlink ref="A66" r:id="rId42" display="https://www.worldometers.info/coronavirus/country/uk/" xr:uid="{9E857743-3BA1-D547-A532-A53EF891F862}"/>
+    <hyperlink ref="A67" r:id="rId43" display="https://www.worldometers.info/coronavirus/country/netherlands/" xr:uid="{AC91BAEF-3072-5948-8933-952BC3477BC0}"/>
     <hyperlink ref="A73" r:id="rId44" display="https://www.worldometers.info/coronavirus/country/austria/" xr:uid="{76C0B263-3E56-DD44-BF90-D7A725F4C11B}"/>
     <hyperlink ref="A64" r:id="rId45" display="https://www.worldometers.info/coronavirus/country/belgium/" xr:uid="{F788A2F0-F76C-0A46-84F6-32311CDCE6EB}"/>
     <hyperlink ref="A75" r:id="rId46" display="https://www.worldometers.info/coronavirus/country/norway/" xr:uid="{1FA4FB2B-21FB-A240-B716-855DE4CC3FCA}"/>

</xml_diff>

<commit_message>
update 13 April II
</commit_message>
<xml_diff>
--- a/COVID19 calculos.xlsx
+++ b/COVID19 calculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rramirez/projects/COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3373AE-6F93-CA4D-85BB-55B88897A3F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F60949E-B938-6142-AA21-0B1EFF55734F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{88028D00-68CA-7A4C-80F7-F9DFC90D5C6B}"/>
   </bookViews>
@@ -10162,7 +10162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F3BD7B-3B40-A94B-99F4-AAD0A2BEB996}">
   <dimension ref="A1:AR80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W48" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AN65" sqref="AN65"/>
     </sheetView>
   </sheetViews>

</xml_diff>